<commit_message>
feat(Trello-45): Add page numbers to footer
</commit_message>
<xml_diff>
--- a/public/templates/ept_tb_submission_form_1.3.xlsx
+++ b/public/templates/ept_tb_submission_form_1.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brich\projects\SystemOne\ept\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28712FAA-3791-45C8-84AF-2CF0A3CDCAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD9D269-7FE7-4956-AA2E-D72C294364FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1284,14 +1284,20 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1302,97 +1308,19 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1466,6 +1394,78 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7442,8 +7442,8 @@
   </sheetPr>
   <dimension ref="A1:Y1342"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A30" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection sqref="A1:W47"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="W1" sqref="A1:W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7464,33 +7464,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="160" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="107" t="s">
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="161" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="119" t="s">
+      <c r="L1" s="161"/>
+      <c r="M1" s="161"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="162"/>
+      <c r="P1" s="162"/>
+      <c r="Q1" s="162"/>
+      <c r="R1" s="162"/>
+      <c r="S1" s="166" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
       <c r="V1" s="99"/>
       <c r="W1" s="99"/>
       <c r="X1" s="76"/>
@@ -7524,91 +7524,91 @@
       <c r="Y2" s="77"/>
     </row>
     <row r="3" spans="1:25" s="1" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="120" t="s">
+      <c r="A3" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="120"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
-      <c r="G3" s="120"/>
-      <c r="H3" s="120"/>
-      <c r="I3" s="120"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="120"/>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="120"/>
-      <c r="O3" s="120"/>
-      <c r="P3" s="120"/>
-      <c r="Q3" s="120"/>
-      <c r="R3" s="120"/>
-      <c r="S3" s="120"/>
-      <c r="T3" s="120"/>
-      <c r="U3" s="120"/>
-      <c r="V3" s="120"/>
-      <c r="W3" s="120"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="106"/>
+      <c r="J3" s="106"/>
+      <c r="K3" s="106"/>
+      <c r="L3" s="106"/>
+      <c r="M3" s="106"/>
+      <c r="N3" s="106"/>
+      <c r="O3" s="106"/>
+      <c r="P3" s="106"/>
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106"/>
+      <c r="S3" s="106"/>
+      <c r="T3" s="106"/>
+      <c r="U3" s="106"/>
+      <c r="V3" s="106"/>
+      <c r="W3" s="106"/>
       <c r="X3" s="25"/>
       <c r="Y3" s="76"/>
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="120"/>
-      <c r="M4" s="120"/>
-      <c r="N4" s="120"/>
-      <c r="O4" s="120"/>
-      <c r="P4" s="120"/>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="120"/>
-      <c r="S4" s="120"/>
-      <c r="T4" s="120"/>
-      <c r="U4" s="120"/>
-      <c r="V4" s="120"/>
-      <c r="W4" s="120"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
+      <c r="M4" s="106"/>
+      <c r="N4" s="106"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106"/>
+      <c r="R4" s="106"/>
+      <c r="S4" s="106"/>
+      <c r="T4" s="106"/>
+      <c r="U4" s="106"/>
+      <c r="V4" s="106"/>
+      <c r="W4" s="106"/>
       <c r="X4" s="27"/>
       <c r="Y4" s="76"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
-      <c r="G5" s="142"/>
-      <c r="H5" s="142"/>
-      <c r="I5" s="142"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="142"/>
-      <c r="L5" s="142"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
       <c r="M5" s="104"/>
       <c r="N5" s="22"/>
-      <c r="O5" s="109" t="s">
+      <c r="O5" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="109" t="s">
+      <c r="P5" s="112"/>
+      <c r="Q5" s="112"/>
+      <c r="R5" s="113"/>
+      <c r="S5" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="110"/>
-      <c r="W5" s="111"/>
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="V5" s="112"/>
+      <c r="W5" s="113"/>
       <c r="X5" s="78"/>
       <c r="Y5" s="79"/>
     </row>
@@ -7627,33 +7627,33 @@
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="113"/>
-      <c r="Q6" s="113"/>
-      <c r="R6" s="114"/>
-      <c r="S6" s="143"/>
-      <c r="T6" s="144"/>
-      <c r="U6" s="144"/>
-      <c r="V6" s="144"/>
-      <c r="W6" s="145"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="114"/>
+      <c r="Q6" s="114"/>
+      <c r="R6" s="115"/>
+      <c r="S6" s="119"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="120"/>
+      <c r="W6" s="121"/>
       <c r="X6" s="78"/>
       <c r="Y6" s="79"/>
     </row>
     <row r="7" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="111" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="126"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
-      <c r="J7" s="142"/>
-      <c r="K7" s="142"/>
-      <c r="L7" s="142"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
       <c r="M7" s="103"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -7683,50 +7683,50 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="146" t="s">
+      <c r="O8" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="147"/>
-      <c r="Q8" s="147"/>
-      <c r="R8" s="147"/>
-      <c r="S8" s="148"/>
-      <c r="T8" s="155"/>
-      <c r="U8" s="156"/>
-      <c r="V8" s="156"/>
-      <c r="W8" s="157"/>
+      <c r="P8" s="123"/>
+      <c r="Q8" s="123"/>
+      <c r="R8" s="123"/>
+      <c r="S8" s="124"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="133"/>
       <c r="X8" s="75"/>
       <c r="Y8" s="25"/>
     </row>
     <row r="9" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="142"/>
-      <c r="E9" s="142"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="142"/>
-      <c r="H9" s="142"/>
-      <c r="I9" s="142"/>
-      <c r="J9" s="142"/>
-      <c r="K9" s="142"/>
-      <c r="L9" s="142"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="117"/>
+      <c r="J9" s="117"/>
+      <c r="K9" s="117"/>
+      <c r="L9" s="117"/>
       <c r="M9" s="103"/>
       <c r="N9" s="22"/>
-      <c r="O9" s="149" t="s">
+      <c r="O9" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="P9" s="150"/>
-      <c r="Q9" s="150"/>
-      <c r="R9" s="150"/>
-      <c r="S9" s="151"/>
-      <c r="T9" s="164" t="s">
+      <c r="P9" s="126"/>
+      <c r="Q9" s="126"/>
+      <c r="R9" s="126"/>
+      <c r="S9" s="127"/>
+      <c r="T9" s="140" t="s">
         <v>55</v>
       </c>
-      <c r="U9" s="165"/>
-      <c r="V9" s="165"/>
-      <c r="W9" s="166"/>
+      <c r="U9" s="141"/>
+      <c r="V9" s="141"/>
+      <c r="W9" s="142"/>
       <c r="X9" s="75"/>
       <c r="Y9" s="12"/>
     </row>
@@ -7745,48 +7745,48 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
-      <c r="O10" s="149" t="s">
+      <c r="O10" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="P10" s="150"/>
-      <c r="Q10" s="150"/>
-      <c r="R10" s="150"/>
-      <c r="S10" s="151"/>
-      <c r="T10" s="158"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="160"/>
+      <c r="P10" s="126"/>
+      <c r="Q10" s="126"/>
+      <c r="R10" s="126"/>
+      <c r="S10" s="127"/>
+      <c r="T10" s="134"/>
+      <c r="U10" s="135"/>
+      <c r="V10" s="135"/>
+      <c r="W10" s="136"/>
       <c r="X10" s="22"/>
       <c r="Y10" s="5"/>
     </row>
     <row r="11" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="111"/>
-      <c r="C11" s="141"/>
-      <c r="D11" s="142"/>
-      <c r="E11" s="142"/>
-      <c r="F11" s="142"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="142"/>
-      <c r="I11" s="142"/>
-      <c r="J11" s="142"/>
-      <c r="K11" s="142"/>
-      <c r="L11" s="142"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="117"/>
+      <c r="K11" s="117"/>
+      <c r="L11" s="117"/>
       <c r="M11" s="103"/>
       <c r="N11" s="22"/>
-      <c r="O11" s="152" t="s">
+      <c r="O11" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="P11" s="153"/>
-      <c r="Q11" s="153"/>
-      <c r="R11" s="153"/>
-      <c r="S11" s="154"/>
-      <c r="T11" s="161"/>
-      <c r="U11" s="162"/>
-      <c r="V11" s="162"/>
-      <c r="W11" s="163"/>
+      <c r="P11" s="129"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
+      <c r="S11" s="130"/>
+      <c r="T11" s="137"/>
+      <c r="U11" s="138"/>
+      <c r="V11" s="138"/>
+      <c r="W11" s="139"/>
       <c r="X11" s="22"/>
       <c r="Y11" s="13"/>
     </row>
@@ -7818,37 +7818,37 @@
       <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:25" ht="31.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="130"/>
-      <c r="B13" s="131"/>
-      <c r="C13" s="127" t="s">
+      <c r="A13" s="148"/>
+      <c r="B13" s="149"/>
+      <c r="C13" s="145" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="128"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="136" t="s">
+      <c r="D13" s="146"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="137"/>
-      <c r="K13" s="137"/>
-      <c r="L13" s="137"/>
-      <c r="M13" s="138" t="s">
+      <c r="J13" s="155"/>
+      <c r="K13" s="155"/>
+      <c r="L13" s="155"/>
+      <c r="M13" s="107" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="139"/>
-      <c r="O13" s="139"/>
-      <c r="P13" s="140"/>
-      <c r="Q13" s="132" t="s">
+      <c r="N13" s="108"/>
+      <c r="O13" s="108"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="R13" s="133"/>
-      <c r="S13" s="133"/>
-      <c r="T13" s="133"/>
-      <c r="U13" s="133"/>
-      <c r="V13" s="133"/>
-      <c r="W13" s="134"/>
+      <c r="R13" s="151"/>
+      <c r="S13" s="151"/>
+      <c r="T13" s="151"/>
+      <c r="U13" s="151"/>
+      <c r="V13" s="151"/>
+      <c r="W13" s="152"/>
       <c r="X13" s="79"/>
       <c r="Y13" s="25"/>
     </row>
@@ -8133,10 +8133,10 @@
       <c r="Y21" s="12"/>
     </row>
     <row r="22" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="135" t="s">
+      <c r="A22" s="153" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="135"/>
+      <c r="B22" s="153"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
@@ -8216,27 +8216,27 @@
       <c r="Y24" s="12"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="117" t="s">
+      <c r="A25" s="164" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
-      <c r="E25" s="117"/>
-      <c r="F25" s="117"/>
-      <c r="G25" s="117"/>
-      <c r="H25" s="117"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="117"/>
-      <c r="K25" s="117"/>
-      <c r="L25" s="117"/>
-      <c r="M25" s="117"/>
-      <c r="N25" s="117"/>
-      <c r="O25" s="117"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="117"/>
-      <c r="R25" s="117"/>
-      <c r="S25" s="117"/>
+      <c r="B25" s="164"/>
+      <c r="C25" s="164"/>
+      <c r="D25" s="164"/>
+      <c r="E25" s="164"/>
+      <c r="F25" s="164"/>
+      <c r="G25" s="164"/>
+      <c r="H25" s="164"/>
+      <c r="I25" s="164"/>
+      <c r="J25" s="164"/>
+      <c r="K25" s="164"/>
+      <c r="L25" s="164"/>
+      <c r="M25" s="164"/>
+      <c r="N25" s="164"/>
+      <c r="O25" s="164"/>
+      <c r="P25" s="164"/>
+      <c r="Q25" s="164"/>
+      <c r="R25" s="164"/>
+      <c r="S25" s="164"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -8245,25 +8245,25 @@
       <c r="Y25" s="3"/>
     </row>
     <row r="26" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="118"/>
-      <c r="B26" s="118"/>
-      <c r="C26" s="118"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="118"/>
-      <c r="F26" s="118"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="118"/>
-      <c r="K26" s="118"/>
-      <c r="L26" s="118"/>
-      <c r="M26" s="118"/>
-      <c r="N26" s="118"/>
-      <c r="O26" s="118"/>
-      <c r="P26" s="118"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="118"/>
-      <c r="S26" s="118"/>
+      <c r="A26" s="165"/>
+      <c r="B26" s="165"/>
+      <c r="C26" s="165"/>
+      <c r="D26" s="165"/>
+      <c r="E26" s="165"/>
+      <c r="F26" s="165"/>
+      <c r="G26" s="165"/>
+      <c r="H26" s="165"/>
+      <c r="I26" s="165"/>
+      <c r="J26" s="165"/>
+      <c r="K26" s="165"/>
+      <c r="L26" s="165"/>
+      <c r="M26" s="165"/>
+      <c r="N26" s="165"/>
+      <c r="O26" s="165"/>
+      <c r="P26" s="165"/>
+      <c r="Q26" s="165"/>
+      <c r="R26" s="165"/>
+      <c r="S26" s="165"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="7"/>
@@ -8301,8 +8301,8 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
-      <c r="B28" s="116"/>
+      <c r="A28" s="110"/>
+      <c r="B28" s="110"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -8328,33 +8328,33 @@
       <c r="Y28" s="7"/>
     </row>
     <row r="29" spans="1:25" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="110"/>
-      <c r="C29" s="110"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="113"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="113"/>
-      <c r="J29" s="113"/>
-      <c r="K29" s="113"/>
-      <c r="L29" s="113"/>
-      <c r="M29" s="114"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="113"/>
+      <c r="F29" s="118"/>
+      <c r="G29" s="114"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="115"/>
       <c r="N29" s="22"/>
-      <c r="O29" s="115" t="s">
+      <c r="O29" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="P29" s="115"/>
-      <c r="Q29" s="115"/>
-      <c r="R29" s="115"/>
-      <c r="S29" s="115"/>
-      <c r="T29" s="115"/>
-      <c r="U29" s="115"/>
-      <c r="V29" s="115"/>
-      <c r="W29" s="115"/>
+      <c r="P29" s="163"/>
+      <c r="Q29" s="163"/>
+      <c r="R29" s="163"/>
+      <c r="S29" s="163"/>
+      <c r="T29" s="163"/>
+      <c r="U29" s="163"/>
+      <c r="V29" s="163"/>
+      <c r="W29" s="163"/>
       <c r="X29" s="78"/>
       <c r="Y29" s="79"/>
     </row>
@@ -8373,44 +8373,44 @@
       <c r="L30" s="23"/>
       <c r="M30" s="23"/>
       <c r="N30" s="23"/>
-      <c r="O30" s="115"/>
-      <c r="P30" s="115"/>
-      <c r="Q30" s="115"/>
-      <c r="R30" s="115"/>
-      <c r="S30" s="115"/>
-      <c r="T30" s="115"/>
-      <c r="U30" s="115"/>
-      <c r="V30" s="115"/>
-      <c r="W30" s="115"/>
+      <c r="O30" s="163"/>
+      <c r="P30" s="163"/>
+      <c r="Q30" s="163"/>
+      <c r="R30" s="163"/>
+      <c r="S30" s="163"/>
+      <c r="T30" s="163"/>
+      <c r="U30" s="163"/>
+      <c r="V30" s="163"/>
+      <c r="W30" s="163"/>
       <c r="X30" s="78"/>
       <c r="Y30" s="79"/>
     </row>
     <row r="31" spans="1:25" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="109" t="s">
+      <c r="A31" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="110"/>
-      <c r="C31" s="110"/>
-      <c r="D31" s="110"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="113"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="113"/>
-      <c r="J31" s="113"/>
-      <c r="K31" s="113"/>
-      <c r="L31" s="113"/>
-      <c r="M31" s="114"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="113"/>
+      <c r="F31" s="114"/>
+      <c r="G31" s="114"/>
+      <c r="H31" s="114"/>
+      <c r="I31" s="114"/>
+      <c r="J31" s="114"/>
+      <c r="K31" s="114"/>
+      <c r="L31" s="114"/>
+      <c r="M31" s="115"/>
       <c r="N31" s="22"/>
-      <c r="O31" s="115"/>
-      <c r="P31" s="115"/>
-      <c r="Q31" s="115"/>
-      <c r="R31" s="115"/>
-      <c r="S31" s="115"/>
-      <c r="T31" s="115"/>
-      <c r="U31" s="115"/>
-      <c r="V31" s="115"/>
-      <c r="W31" s="115"/>
+      <c r="O31" s="163"/>
+      <c r="P31" s="163"/>
+      <c r="Q31" s="163"/>
+      <c r="R31" s="163"/>
+      <c r="S31" s="163"/>
+      <c r="T31" s="163"/>
+      <c r="U31" s="163"/>
+      <c r="V31" s="163"/>
+      <c r="W31" s="163"/>
       <c r="X31" s="24"/>
       <c r="Y31" s="12"/>
     </row>
@@ -8429,50 +8429,50 @@
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
-      <c r="O32" s="115"/>
-      <c r="P32" s="115"/>
-      <c r="Q32" s="115"/>
-      <c r="R32" s="115"/>
-      <c r="S32" s="115"/>
-      <c r="T32" s="115"/>
-      <c r="U32" s="115"/>
-      <c r="V32" s="115"/>
-      <c r="W32" s="115"/>
+      <c r="O32" s="163"/>
+      <c r="P32" s="163"/>
+      <c r="Q32" s="163"/>
+      <c r="R32" s="163"/>
+      <c r="S32" s="163"/>
+      <c r="T32" s="163"/>
+      <c r="U32" s="163"/>
+      <c r="V32" s="163"/>
+      <c r="W32" s="163"/>
       <c r="X32" s="75"/>
       <c r="Y32" s="25"/>
     </row>
     <row r="33" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="109" t="s">
+      <c r="A33" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="110"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="111"/>
-      <c r="F33" s="113"/>
-      <c r="G33" s="113"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="113"/>
-      <c r="J33" s="113"/>
-      <c r="K33" s="113"/>
-      <c r="L33" s="113"/>
-      <c r="M33" s="114"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="113"/>
+      <c r="F33" s="114"/>
+      <c r="G33" s="114"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="114"/>
+      <c r="J33" s="114"/>
+      <c r="K33" s="114"/>
+      <c r="L33" s="114"/>
+      <c r="M33" s="115"/>
       <c r="N33" s="22"/>
-      <c r="O33" s="115"/>
-      <c r="P33" s="115"/>
-      <c r="Q33" s="115"/>
-      <c r="R33" s="115"/>
-      <c r="S33" s="115"/>
-      <c r="T33" s="115"/>
-      <c r="U33" s="115"/>
-      <c r="V33" s="115"/>
-      <c r="W33" s="115"/>
+      <c r="O33" s="163"/>
+      <c r="P33" s="163"/>
+      <c r="Q33" s="163"/>
+      <c r="R33" s="163"/>
+      <c r="S33" s="163"/>
+      <c r="T33" s="163"/>
+      <c r="U33" s="163"/>
+      <c r="V33" s="163"/>
+      <c r="W33" s="163"/>
       <c r="X33" s="22"/>
       <c r="Y33" s="13"/>
     </row>
     <row r="34" spans="1:25" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="116"/>
-      <c r="B34" s="116"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -8485,46 +8485,46 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="115"/>
-      <c r="P34" s="115"/>
-      <c r="Q34" s="115"/>
-      <c r="R34" s="115"/>
-      <c r="S34" s="115"/>
-      <c r="T34" s="115"/>
-      <c r="U34" s="115"/>
-      <c r="V34" s="115"/>
-      <c r="W34" s="115"/>
+      <c r="O34" s="163"/>
+      <c r="P34" s="163"/>
+      <c r="Q34" s="163"/>
+      <c r="R34" s="163"/>
+      <c r="S34" s="163"/>
+      <c r="T34" s="163"/>
+      <c r="U34" s="163"/>
+      <c r="V34" s="163"/>
+      <c r="W34" s="163"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="7"/>
     </row>
     <row r="35" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="111" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="110"/>
-      <c r="C35" s="110"/>
-      <c r="D35" s="110"/>
-      <c r="E35" s="111"/>
-      <c r="F35" s="113" t="s">
+      <c r="B35" s="112"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="114"/>
+      <c r="G35" s="114"/>
+      <c r="H35" s="114"/>
+      <c r="I35" s="114"/>
+      <c r="J35" s="114"/>
+      <c r="K35" s="114"/>
+      <c r="L35" s="114"/>
+      <c r="M35" s="115"/>
       <c r="N35" s="22"/>
-      <c r="O35" s="115"/>
-      <c r="P35" s="115"/>
-      <c r="Q35" s="115"/>
-      <c r="R35" s="115"/>
-      <c r="S35" s="115"/>
-      <c r="T35" s="115"/>
-      <c r="U35" s="115"/>
-      <c r="V35" s="115"/>
-      <c r="W35" s="115"/>
+      <c r="O35" s="163"/>
+      <c r="P35" s="163"/>
+      <c r="Q35" s="163"/>
+      <c r="R35" s="163"/>
+      <c r="S35" s="163"/>
+      <c r="T35" s="163"/>
+      <c r="U35" s="163"/>
+      <c r="V35" s="163"/>
+      <c r="W35" s="163"/>
       <c r="X35" s="75"/>
       <c r="Y35" s="12"/>
     </row>
@@ -8543,36 +8543,36 @@
       <c r="L36" s="23"/>
       <c r="M36" s="23"/>
       <c r="N36" s="23"/>
-      <c r="O36" s="115"/>
-      <c r="P36" s="115"/>
-      <c r="Q36" s="115"/>
-      <c r="R36" s="115"/>
-      <c r="S36" s="115"/>
-      <c r="T36" s="115"/>
-      <c r="U36" s="115"/>
-      <c r="V36" s="115"/>
-      <c r="W36" s="115"/>
+      <c r="O36" s="163"/>
+      <c r="P36" s="163"/>
+      <c r="Q36" s="163"/>
+      <c r="R36" s="163"/>
+      <c r="S36" s="163"/>
+      <c r="T36" s="163"/>
+      <c r="U36" s="163"/>
+      <c r="V36" s="163"/>
+      <c r="W36" s="163"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="5"/>
     </row>
     <row r="37" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="109" t="s">
+      <c r="A37" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="110"/>
-      <c r="C37" s="110"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="113" t="s">
+      <c r="B37" s="112"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="114" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="113"/>
-      <c r="H37" s="113"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="113"/>
-      <c r="K37" s="113"/>
-      <c r="L37" s="113"/>
-      <c r="M37" s="114"/>
+      <c r="G37" s="114"/>
+      <c r="H37" s="114"/>
+      <c r="I37" s="114"/>
+      <c r="J37" s="114"/>
+      <c r="K37" s="114"/>
+      <c r="L37" s="114"/>
+      <c r="M37" s="115"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
       <c r="P37" s="100"/>
@@ -8614,21 +8614,21 @@
       <c r="Y38" s="5"/>
     </row>
     <row r="39" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="109" t="s">
+      <c r="A39" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="110"/>
-      <c r="C39" s="110"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="111"/>
-      <c r="F39" s="112"/>
-      <c r="G39" s="113"/>
-      <c r="H39" s="113"/>
-      <c r="I39" s="113"/>
-      <c r="J39" s="113"/>
-      <c r="K39" s="113"/>
-      <c r="L39" s="113"/>
-      <c r="M39" s="114"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="113"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="114"/>
+      <c r="H39" s="114"/>
+      <c r="I39" s="114"/>
+      <c r="J39" s="114"/>
+      <c r="K39" s="114"/>
+      <c r="L39" s="114"/>
+      <c r="M39" s="115"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
       <c r="P39" s="90"/>
@@ -8643,8 +8643,8 @@
       <c r="Y39" s="13"/>
     </row>
     <row r="40" spans="1:25" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="116"/>
-      <c r="B40" s="116"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -8670,21 +8670,21 @@
       <c r="Y40" s="6"/>
     </row>
     <row r="41" spans="1:25" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="109" t="s">
+      <c r="A41" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="110"/>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="111"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="113"/>
-      <c r="H41" s="113"/>
-      <c r="I41" s="113"/>
-      <c r="J41" s="113"/>
-      <c r="K41" s="113"/>
-      <c r="L41" s="113"/>
-      <c r="M41" s="114"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="113"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="114"/>
+      <c r="H41" s="114"/>
+      <c r="I41" s="114"/>
+      <c r="J41" s="114"/>
+      <c r="K41" s="114"/>
+      <c r="L41" s="114"/>
+      <c r="M41" s="115"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
       <c r="P41" s="90"/>
@@ -8726,21 +8726,21 @@
       <c r="Y42" s="79"/>
     </row>
     <row r="43" spans="1:25" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="109" t="s">
+      <c r="A43" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="110"/>
-      <c r="C43" s="110"/>
-      <c r="D43" s="110"/>
-      <c r="E43" s="111"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="113"/>
-      <c r="H43" s="113"/>
-      <c r="I43" s="113"/>
-      <c r="J43" s="113"/>
-      <c r="K43" s="113"/>
-      <c r="L43" s="113"/>
-      <c r="M43" s="114"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="118"/>
+      <c r="G43" s="114"/>
+      <c r="H43" s="114"/>
+      <c r="I43" s="114"/>
+      <c r="J43" s="114"/>
+      <c r="K43" s="114"/>
+      <c r="L43" s="114"/>
+      <c r="M43" s="115"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
       <c r="P43" s="90"/>
@@ -8782,23 +8782,23 @@
       <c r="Y44" s="25"/>
     </row>
     <row r="45" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="109" t="s">
+      <c r="A45" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="110"/>
-      <c r="C45" s="110"/>
-      <c r="D45" s="110"/>
-      <c r="E45" s="111"/>
-      <c r="F45" s="113" t="s">
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="113"/>
+      <c r="F45" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="113"/>
-      <c r="H45" s="113"/>
-      <c r="I45" s="113"/>
-      <c r="J45" s="113"/>
-      <c r="K45" s="113"/>
-      <c r="L45" s="113"/>
-      <c r="M45" s="114"/>
+      <c r="G45" s="114"/>
+      <c r="H45" s="114"/>
+      <c r="I45" s="114"/>
+      <c r="J45" s="114"/>
+      <c r="K45" s="114"/>
+      <c r="L45" s="114"/>
+      <c r="M45" s="115"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
       <c r="P45" s="90"/>
@@ -8840,21 +8840,21 @@
       <c r="Y46" s="25"/>
     </row>
     <row r="47" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="109" t="s">
+      <c r="A47" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="110"/>
-      <c r="C47" s="110"/>
-      <c r="D47" s="110"/>
-      <c r="E47" s="111"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="113"/>
-      <c r="H47" s="113"/>
-      <c r="I47" s="113"/>
-      <c r="J47" s="113"/>
-      <c r="K47" s="113"/>
-      <c r="L47" s="113"/>
-      <c r="M47" s="114"/>
+      <c r="B47" s="112"/>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="113"/>
+      <c r="F47" s="114"/>
+      <c r="G47" s="114"/>
+      <c r="H47" s="114"/>
+      <c r="I47" s="114"/>
+      <c r="J47" s="114"/>
+      <c r="K47" s="114"/>
+      <c r="L47" s="114"/>
+      <c r="M47" s="115"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
       <c r="P47" s="90"/>
@@ -8869,8 +8869,8 @@
       <c r="Y47" s="13"/>
     </row>
     <row r="48" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="125"/>
-      <c r="B48" s="125"/>
+      <c r="A48" s="143"/>
+      <c r="B48" s="143"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -8976,8 +8976,8 @@
       <c r="Y51" s="85"/>
     </row>
     <row r="52" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="122"/>
-      <c r="B52" s="122"/>
+      <c r="A52" s="156"/>
+      <c r="B52" s="156"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -9003,8 +9003,8 @@
       <c r="Y52" s="5"/>
     </row>
     <row r="53" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="122"/>
-      <c r="B53" s="122"/>
+      <c r="A53" s="156"/>
+      <c r="B53" s="156"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -9030,8 +9030,8 @@
       <c r="Y53" s="6"/>
     </row>
     <row r="54" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="116"/>
-      <c r="B54" s="116"/>
+      <c r="A54" s="110"/>
+      <c r="B54" s="110"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -9057,8 +9057,8 @@
       <c r="Y54" s="6"/>
     </row>
     <row r="55" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="116"/>
-      <c r="B55" s="116"/>
+      <c r="A55" s="110"/>
+      <c r="B55" s="110"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -9084,8 +9084,8 @@
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="116"/>
-      <c r="B56" s="116"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="110"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -9111,8 +9111,8 @@
       <c r="Y56" s="6"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A57" s="116"/>
-      <c r="B57" s="116"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="110"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -9192,35 +9192,35 @@
       <c r="Y59" s="4"/>
     </row>
     <row r="60" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="123"/>
-      <c r="B60" s="123"/>
-      <c r="C60" s="121"/>
-      <c r="D60" s="121"/>
-      <c r="E60" s="121"/>
-      <c r="F60" s="121"/>
-      <c r="G60" s="121"/>
-      <c r="H60" s="121"/>
-      <c r="I60" s="121"/>
-      <c r="J60" s="121"/>
-      <c r="K60" s="121"/>
-      <c r="L60" s="121"/>
-      <c r="M60" s="121"/>
-      <c r="N60" s="121"/>
-      <c r="O60" s="121"/>
-      <c r="P60" s="121"/>
-      <c r="Q60" s="121"/>
-      <c r="R60" s="121"/>
-      <c r="S60" s="121"/>
-      <c r="T60" s="121"/>
-      <c r="U60" s="121"/>
-      <c r="V60" s="121"/>
-      <c r="W60" s="121"/>
-      <c r="X60" s="121"/>
-      <c r="Y60" s="121"/>
+      <c r="A60" s="158"/>
+      <c r="B60" s="158"/>
+      <c r="C60" s="157"/>
+      <c r="D60" s="157"/>
+      <c r="E60" s="157"/>
+      <c r="F60" s="157"/>
+      <c r="G60" s="157"/>
+      <c r="H60" s="157"/>
+      <c r="I60" s="157"/>
+      <c r="J60" s="157"/>
+      <c r="K60" s="157"/>
+      <c r="L60" s="157"/>
+      <c r="M60" s="157"/>
+      <c r="N60" s="157"/>
+      <c r="O60" s="157"/>
+      <c r="P60" s="157"/>
+      <c r="Q60" s="157"/>
+      <c r="R60" s="157"/>
+      <c r="S60" s="157"/>
+      <c r="T60" s="157"/>
+      <c r="U60" s="157"/>
+      <c r="V60" s="157"/>
+      <c r="W60" s="157"/>
+      <c r="X60" s="157"/>
+      <c r="Y60" s="157"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A61" s="122"/>
-      <c r="B61" s="122"/>
+      <c r="A61" s="156"/>
+      <c r="B61" s="156"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -9246,8 +9246,8 @@
       <c r="Y61" s="5"/>
     </row>
     <row r="62" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="122"/>
-      <c r="B62" s="122"/>
+      <c r="A62" s="156"/>
+      <c r="B62" s="156"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -9273,8 +9273,8 @@
       <c r="Y62" s="6"/>
     </row>
     <row r="63" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="116"/>
-      <c r="B63" s="116"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="110"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -9300,8 +9300,8 @@
       <c r="Y63" s="6"/>
     </row>
     <row r="64" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="116"/>
-      <c r="B64" s="116"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="110"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
@@ -9327,8 +9327,8 @@
       <c r="Y64" s="7"/>
     </row>
     <row r="65" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="116"/>
-      <c r="B65" s="116"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="110"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -9354,8 +9354,8 @@
       <c r="Y65" s="6"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A66" s="116"/>
-      <c r="B66" s="116"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="110"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -9489,35 +9489,35 @@
       <c r="Y70" s="4"/>
     </row>
     <row r="71" spans="1:25" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="124"/>
-      <c r="B71" s="124"/>
-      <c r="C71" s="121"/>
-      <c r="D71" s="121"/>
-      <c r="E71" s="121"/>
-      <c r="F71" s="121"/>
-      <c r="G71" s="121"/>
-      <c r="H71" s="121"/>
-      <c r="I71" s="121"/>
-      <c r="J71" s="121"/>
-      <c r="K71" s="121"/>
-      <c r="L71" s="121"/>
-      <c r="M71" s="121"/>
-      <c r="N71" s="121"/>
-      <c r="O71" s="121"/>
-      <c r="P71" s="121"/>
-      <c r="Q71" s="121"/>
-      <c r="R71" s="121"/>
-      <c r="S71" s="121"/>
-      <c r="T71" s="121"/>
-      <c r="U71" s="121"/>
-      <c r="V71" s="121"/>
-      <c r="W71" s="121"/>
-      <c r="X71" s="121"/>
-      <c r="Y71" s="121"/>
+      <c r="A71" s="159"/>
+      <c r="B71" s="159"/>
+      <c r="C71" s="157"/>
+      <c r="D71" s="157"/>
+      <c r="E71" s="157"/>
+      <c r="F71" s="157"/>
+      <c r="G71" s="157"/>
+      <c r="H71" s="157"/>
+      <c r="I71" s="157"/>
+      <c r="J71" s="157"/>
+      <c r="K71" s="157"/>
+      <c r="L71" s="157"/>
+      <c r="M71" s="157"/>
+      <c r="N71" s="157"/>
+      <c r="O71" s="157"/>
+      <c r="P71" s="157"/>
+      <c r="Q71" s="157"/>
+      <c r="R71" s="157"/>
+      <c r="S71" s="157"/>
+      <c r="T71" s="157"/>
+      <c r="U71" s="157"/>
+      <c r="V71" s="157"/>
+      <c r="W71" s="157"/>
+      <c r="X71" s="157"/>
+      <c r="Y71" s="157"/>
     </row>
     <row r="72" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="122"/>
-      <c r="B72" s="122"/>
+      <c r="A72" s="156"/>
+      <c r="B72" s="156"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -9543,8 +9543,8 @@
       <c r="Y72" s="5"/>
     </row>
     <row r="73" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="122"/>
-      <c r="B73" s="122"/>
+      <c r="A73" s="156"/>
+      <c r="B73" s="156"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -9570,8 +9570,8 @@
       <c r="Y73" s="9"/>
     </row>
     <row r="74" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="116"/>
-      <c r="B74" s="116"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="110"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -9597,8 +9597,8 @@
       <c r="Y74" s="9"/>
     </row>
     <row r="75" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="116"/>
-      <c r="B75" s="116"/>
+      <c r="A75" s="110"/>
+      <c r="B75" s="110"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -9624,8 +9624,8 @@
       <c r="Y75" s="10"/>
     </row>
     <row r="76" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="116"/>
-      <c r="B76" s="116"/>
+      <c r="A76" s="110"/>
+      <c r="B76" s="110"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -9651,8 +9651,8 @@
       <c r="Y76" s="9"/>
     </row>
     <row r="77" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="116"/>
-      <c r="B77" s="116"/>
+      <c r="A77" s="110"/>
+      <c r="B77" s="110"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -9732,35 +9732,35 @@
       <c r="Y79" s="4"/>
     </row>
     <row r="80" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="123"/>
-      <c r="B80" s="123"/>
-      <c r="C80" s="121"/>
-      <c r="D80" s="121"/>
-      <c r="E80" s="121"/>
-      <c r="F80" s="121"/>
-      <c r="G80" s="121"/>
-      <c r="H80" s="121"/>
-      <c r="I80" s="121"/>
-      <c r="J80" s="121"/>
-      <c r="K80" s="121"/>
-      <c r="L80" s="121"/>
-      <c r="M80" s="121"/>
-      <c r="N80" s="121"/>
-      <c r="O80" s="121"/>
-      <c r="P80" s="121"/>
-      <c r="Q80" s="121"/>
-      <c r="R80" s="121"/>
-      <c r="S80" s="121"/>
-      <c r="T80" s="121"/>
-      <c r="U80" s="121"/>
-      <c r="V80" s="121"/>
-      <c r="W80" s="121"/>
-      <c r="X80" s="121"/>
-      <c r="Y80" s="121"/>
+      <c r="A80" s="158"/>
+      <c r="B80" s="158"/>
+      <c r="C80" s="157"/>
+      <c r="D80" s="157"/>
+      <c r="E80" s="157"/>
+      <c r="F80" s="157"/>
+      <c r="G80" s="157"/>
+      <c r="H80" s="157"/>
+      <c r="I80" s="157"/>
+      <c r="J80" s="157"/>
+      <c r="K80" s="157"/>
+      <c r="L80" s="157"/>
+      <c r="M80" s="157"/>
+      <c r="N80" s="157"/>
+      <c r="O80" s="157"/>
+      <c r="P80" s="157"/>
+      <c r="Q80" s="157"/>
+      <c r="R80" s="157"/>
+      <c r="S80" s="157"/>
+      <c r="T80" s="157"/>
+      <c r="U80" s="157"/>
+      <c r="V80" s="157"/>
+      <c r="W80" s="157"/>
+      <c r="X80" s="157"/>
+      <c r="Y80" s="157"/>
     </row>
     <row r="81" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="122"/>
-      <c r="B81" s="122"/>
+      <c r="A81" s="156"/>
+      <c r="B81" s="156"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -9786,8 +9786,8 @@
       <c r="Y81" s="5"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A82" s="122"/>
-      <c r="B82" s="122"/>
+      <c r="A82" s="156"/>
+      <c r="B82" s="156"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
@@ -9813,8 +9813,8 @@
       <c r="Y82" s="6"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A83" s="116"/>
-      <c r="B83" s="116"/>
+      <c r="A83" s="110"/>
+      <c r="B83" s="110"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
@@ -9840,8 +9840,8 @@
       <c r="Y83" s="6"/>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A84" s="116"/>
-      <c r="B84" s="116"/>
+      <c r="A84" s="110"/>
+      <c r="B84" s="110"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -9867,8 +9867,8 @@
       <c r="Y84" s="7"/>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A85" s="116"/>
-      <c r="B85" s="116"/>
+      <c r="A85" s="110"/>
+      <c r="B85" s="110"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
@@ -9894,8 +9894,8 @@
       <c r="Y85" s="6"/>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A86" s="116"/>
-      <c r="B86" s="116"/>
+      <c r="A86" s="110"/>
+      <c r="B86" s="110"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -9975,35 +9975,35 @@
       <c r="Y88" s="4"/>
     </row>
     <row r="89" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="123"/>
-      <c r="B89" s="123"/>
-      <c r="C89" s="121"/>
-      <c r="D89" s="121"/>
-      <c r="E89" s="121"/>
-      <c r="F89" s="121"/>
-      <c r="G89" s="121"/>
-      <c r="H89" s="121"/>
-      <c r="I89" s="121"/>
-      <c r="J89" s="121"/>
-      <c r="K89" s="121"/>
-      <c r="L89" s="121"/>
-      <c r="M89" s="121"/>
-      <c r="N89" s="121"/>
-      <c r="O89" s="121"/>
-      <c r="P89" s="121"/>
-      <c r="Q89" s="121"/>
-      <c r="R89" s="121"/>
-      <c r="S89" s="121"/>
-      <c r="T89" s="121"/>
-      <c r="U89" s="121"/>
-      <c r="V89" s="121"/>
-      <c r="W89" s="121"/>
-      <c r="X89" s="121"/>
-      <c r="Y89" s="121"/>
+      <c r="A89" s="158"/>
+      <c r="B89" s="158"/>
+      <c r="C89" s="157"/>
+      <c r="D89" s="157"/>
+      <c r="E89" s="157"/>
+      <c r="F89" s="157"/>
+      <c r="G89" s="157"/>
+      <c r="H89" s="157"/>
+      <c r="I89" s="157"/>
+      <c r="J89" s="157"/>
+      <c r="K89" s="157"/>
+      <c r="L89" s="157"/>
+      <c r="M89" s="157"/>
+      <c r="N89" s="157"/>
+      <c r="O89" s="157"/>
+      <c r="P89" s="157"/>
+      <c r="Q89" s="157"/>
+      <c r="R89" s="157"/>
+      <c r="S89" s="157"/>
+      <c r="T89" s="157"/>
+      <c r="U89" s="157"/>
+      <c r="V89" s="157"/>
+      <c r="W89" s="157"/>
+      <c r="X89" s="157"/>
+      <c r="Y89" s="157"/>
     </row>
     <row r="90" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="122"/>
-      <c r="B90" s="122"/>
+      <c r="A90" s="156"/>
+      <c r="B90" s="156"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -10029,8 +10029,8 @@
       <c r="Y90" s="5"/>
     </row>
     <row r="91" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="122"/>
-      <c r="B91" s="122"/>
+      <c r="A91" s="156"/>
+      <c r="B91" s="156"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -10056,8 +10056,8 @@
       <c r="Y91" s="9"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A92" s="116"/>
-      <c r="B92" s="116"/>
+      <c r="A92" s="110"/>
+      <c r="B92" s="110"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
@@ -10083,8 +10083,8 @@
       <c r="Y92" s="6"/>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A93" s="116"/>
-      <c r="B93" s="116"/>
+      <c r="A93" s="110"/>
+      <c r="B93" s="110"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -10110,8 +10110,8 @@
       <c r="Y93" s="7"/>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A94" s="116"/>
-      <c r="B94" s="116"/>
+      <c r="A94" s="110"/>
+      <c r="B94" s="110"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
@@ -10137,8 +10137,8 @@
       <c r="Y94" s="6"/>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A95" s="116"/>
-      <c r="B95" s="116"/>
+      <c r="A95" s="110"/>
+      <c r="B95" s="110"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -10245,35 +10245,35 @@
       <c r="Y98" s="7"/>
     </row>
     <row r="99" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="123"/>
-      <c r="B99" s="123"/>
-      <c r="C99" s="121"/>
-      <c r="D99" s="121"/>
-      <c r="E99" s="121"/>
-      <c r="F99" s="121"/>
-      <c r="G99" s="121"/>
-      <c r="H99" s="121"/>
-      <c r="I99" s="121"/>
-      <c r="J99" s="121"/>
-      <c r="K99" s="121"/>
-      <c r="L99" s="121"/>
-      <c r="M99" s="121"/>
-      <c r="N99" s="121"/>
-      <c r="O99" s="121"/>
-      <c r="P99" s="121"/>
-      <c r="Q99" s="121"/>
-      <c r="R99" s="121"/>
-      <c r="S99" s="121"/>
-      <c r="T99" s="121"/>
-      <c r="U99" s="121"/>
-      <c r="V99" s="121"/>
-      <c r="W99" s="121"/>
-      <c r="X99" s="121"/>
-      <c r="Y99" s="121"/>
+      <c r="A99" s="158"/>
+      <c r="B99" s="158"/>
+      <c r="C99" s="157"/>
+      <c r="D99" s="157"/>
+      <c r="E99" s="157"/>
+      <c r="F99" s="157"/>
+      <c r="G99" s="157"/>
+      <c r="H99" s="157"/>
+      <c r="I99" s="157"/>
+      <c r="J99" s="157"/>
+      <c r="K99" s="157"/>
+      <c r="L99" s="157"/>
+      <c r="M99" s="157"/>
+      <c r="N99" s="157"/>
+      <c r="O99" s="157"/>
+      <c r="P99" s="157"/>
+      <c r="Q99" s="157"/>
+      <c r="R99" s="157"/>
+      <c r="S99" s="157"/>
+      <c r="T99" s="157"/>
+      <c r="U99" s="157"/>
+      <c r="V99" s="157"/>
+      <c r="W99" s="157"/>
+      <c r="X99" s="157"/>
+      <c r="Y99" s="157"/>
     </row>
     <row r="100" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="122"/>
-      <c r="B100" s="122"/>
+      <c r="A100" s="156"/>
+      <c r="B100" s="156"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -10299,8 +10299,8 @@
       <c r="Y100" s="5"/>
     </row>
     <row r="101" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="122"/>
-      <c r="B101" s="122"/>
+      <c r="A101" s="156"/>
+      <c r="B101" s="156"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -10326,8 +10326,8 @@
       <c r="Y101" s="9"/>
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A102" s="116"/>
-      <c r="B102" s="116"/>
+      <c r="A102" s="110"/>
+      <c r="B102" s="110"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
@@ -10353,8 +10353,8 @@
       <c r="Y102" s="6"/>
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A103" s="116"/>
-      <c r="B103" s="116"/>
+      <c r="A103" s="110"/>
+      <c r="B103" s="110"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
@@ -10380,8 +10380,8 @@
       <c r="Y103" s="6"/>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A104" s="116"/>
-      <c r="B104" s="116"/>
+      <c r="A104" s="110"/>
+      <c r="B104" s="110"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
@@ -10407,8 +10407,8 @@
       <c r="Y104" s="6"/>
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A105" s="116"/>
-      <c r="B105" s="116"/>
+      <c r="A105" s="110"/>
+      <c r="B105" s="110"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
@@ -10488,35 +10488,35 @@
       <c r="Y107" s="6"/>
     </row>
     <row r="108" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="123"/>
-      <c r="B108" s="123"/>
-      <c r="C108" s="121"/>
-      <c r="D108" s="121"/>
-      <c r="E108" s="121"/>
-      <c r="F108" s="121"/>
-      <c r="G108" s="121"/>
-      <c r="H108" s="121"/>
-      <c r="I108" s="121"/>
-      <c r="J108" s="121"/>
-      <c r="K108" s="121"/>
-      <c r="L108" s="121"/>
-      <c r="M108" s="121"/>
-      <c r="N108" s="121"/>
-      <c r="O108" s="121"/>
-      <c r="P108" s="121"/>
-      <c r="Q108" s="121"/>
-      <c r="R108" s="121"/>
-      <c r="S108" s="121"/>
-      <c r="T108" s="121"/>
-      <c r="U108" s="121"/>
-      <c r="V108" s="121"/>
-      <c r="W108" s="121"/>
-      <c r="X108" s="121"/>
-      <c r="Y108" s="121"/>
+      <c r="A108" s="158"/>
+      <c r="B108" s="158"/>
+      <c r="C108" s="157"/>
+      <c r="D108" s="157"/>
+      <c r="E108" s="157"/>
+      <c r="F108" s="157"/>
+      <c r="G108" s="157"/>
+      <c r="H108" s="157"/>
+      <c r="I108" s="157"/>
+      <c r="J108" s="157"/>
+      <c r="K108" s="157"/>
+      <c r="L108" s="157"/>
+      <c r="M108" s="157"/>
+      <c r="N108" s="157"/>
+      <c r="O108" s="157"/>
+      <c r="P108" s="157"/>
+      <c r="Q108" s="157"/>
+      <c r="R108" s="157"/>
+      <c r="S108" s="157"/>
+      <c r="T108" s="157"/>
+      <c r="U108" s="157"/>
+      <c r="V108" s="157"/>
+      <c r="W108" s="157"/>
+      <c r="X108" s="157"/>
+      <c r="Y108" s="157"/>
     </row>
     <row r="109" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="122"/>
-      <c r="B109" s="122"/>
+      <c r="A109" s="156"/>
+      <c r="B109" s="156"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
@@ -10542,8 +10542,8 @@
       <c r="Y109" s="5"/>
     </row>
     <row r="110" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="122"/>
-      <c r="B110" s="122"/>
+      <c r="A110" s="156"/>
+      <c r="B110" s="156"/>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -10569,8 +10569,8 @@
       <c r="Y110" s="9"/>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A111" s="116"/>
-      <c r="B111" s="116"/>
+      <c r="A111" s="110"/>
+      <c r="B111" s="110"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
@@ -10596,8 +10596,8 @@
       <c r="Y111" s="6"/>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A112" s="116"/>
-      <c r="B112" s="116"/>
+      <c r="A112" s="110"/>
+      <c r="B112" s="110"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
@@ -10623,8 +10623,8 @@
       <c r="Y112" s="6"/>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A113" s="116"/>
-      <c r="B113" s="116"/>
+      <c r="A113" s="110"/>
+      <c r="B113" s="110"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
@@ -10650,8 +10650,8 @@
       <c r="Y113" s="6"/>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A114" s="116"/>
-      <c r="B114" s="116"/>
+      <c r="A114" s="110"/>
+      <c r="B114" s="110"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
@@ -10731,35 +10731,35 @@
       <c r="Y116" s="6"/>
     </row>
     <row r="117" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="123"/>
-      <c r="B117" s="123"/>
-      <c r="C117" s="121"/>
-      <c r="D117" s="121"/>
-      <c r="E117" s="121"/>
-      <c r="F117" s="121"/>
-      <c r="G117" s="121"/>
-      <c r="H117" s="121"/>
-      <c r="I117" s="121"/>
-      <c r="J117" s="121"/>
-      <c r="K117" s="121"/>
-      <c r="L117" s="121"/>
-      <c r="M117" s="121"/>
-      <c r="N117" s="121"/>
-      <c r="O117" s="121"/>
-      <c r="P117" s="121"/>
-      <c r="Q117" s="121"/>
-      <c r="R117" s="121"/>
-      <c r="S117" s="121"/>
-      <c r="T117" s="121"/>
-      <c r="U117" s="121"/>
-      <c r="V117" s="121"/>
-      <c r="W117" s="121"/>
-      <c r="X117" s="121"/>
-      <c r="Y117" s="121"/>
+      <c r="A117" s="158"/>
+      <c r="B117" s="158"/>
+      <c r="C117" s="157"/>
+      <c r="D117" s="157"/>
+      <c r="E117" s="157"/>
+      <c r="F117" s="157"/>
+      <c r="G117" s="157"/>
+      <c r="H117" s="157"/>
+      <c r="I117" s="157"/>
+      <c r="J117" s="157"/>
+      <c r="K117" s="157"/>
+      <c r="L117" s="157"/>
+      <c r="M117" s="157"/>
+      <c r="N117" s="157"/>
+      <c r="O117" s="157"/>
+      <c r="P117" s="157"/>
+      <c r="Q117" s="157"/>
+      <c r="R117" s="157"/>
+      <c r="S117" s="157"/>
+      <c r="T117" s="157"/>
+      <c r="U117" s="157"/>
+      <c r="V117" s="157"/>
+      <c r="W117" s="157"/>
+      <c r="X117" s="157"/>
+      <c r="Y117" s="157"/>
     </row>
     <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="122"/>
-      <c r="B118" s="122"/>
+      <c r="A118" s="156"/>
+      <c r="B118" s="156"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
@@ -10785,8 +10785,8 @@
       <c r="Y118" s="5"/>
     </row>
     <row r="119" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="122"/>
-      <c r="B119" s="122"/>
+      <c r="A119" s="156"/>
+      <c r="B119" s="156"/>
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -10812,8 +10812,8 @@
       <c r="Y119" s="9"/>
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A120" s="116"/>
-      <c r="B120" s="116"/>
+      <c r="A120" s="110"/>
+      <c r="B120" s="110"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
@@ -10839,8 +10839,8 @@
       <c r="Y120" s="6"/>
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A121" s="116"/>
-      <c r="B121" s="116"/>
+      <c r="A121" s="110"/>
+      <c r="B121" s="110"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
@@ -10866,8 +10866,8 @@
       <c r="Y121" s="6"/>
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A122" s="116"/>
-      <c r="B122" s="116"/>
+      <c r="A122" s="110"/>
+      <c r="B122" s="110"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
       <c r="E122" s="6"/>
@@ -10893,8 +10893,8 @@
       <c r="Y122" s="6"/>
     </row>
     <row r="123" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A123" s="116"/>
-      <c r="B123" s="116"/>
+      <c r="A123" s="110"/>
+      <c r="B123" s="110"/>
       <c r="C123" s="6"/>
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
@@ -11001,35 +11001,35 @@
       <c r="Y126" s="6"/>
     </row>
     <row r="127" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="123"/>
-      <c r="B127" s="123"/>
-      <c r="C127" s="121"/>
-      <c r="D127" s="121"/>
-      <c r="E127" s="121"/>
-      <c r="F127" s="121"/>
-      <c r="G127" s="121"/>
-      <c r="H127" s="121"/>
-      <c r="I127" s="121"/>
-      <c r="J127" s="121"/>
-      <c r="K127" s="121"/>
-      <c r="L127" s="121"/>
-      <c r="M127" s="121"/>
-      <c r="N127" s="121"/>
-      <c r="O127" s="121"/>
-      <c r="P127" s="121"/>
-      <c r="Q127" s="121"/>
-      <c r="R127" s="121"/>
-      <c r="S127" s="121"/>
-      <c r="T127" s="121"/>
-      <c r="U127" s="121"/>
-      <c r="V127" s="121"/>
-      <c r="W127" s="121"/>
-      <c r="X127" s="121"/>
-      <c r="Y127" s="121"/>
+      <c r="A127" s="158"/>
+      <c r="B127" s="158"/>
+      <c r="C127" s="157"/>
+      <c r="D127" s="157"/>
+      <c r="E127" s="157"/>
+      <c r="F127" s="157"/>
+      <c r="G127" s="157"/>
+      <c r="H127" s="157"/>
+      <c r="I127" s="157"/>
+      <c r="J127" s="157"/>
+      <c r="K127" s="157"/>
+      <c r="L127" s="157"/>
+      <c r="M127" s="157"/>
+      <c r="N127" s="157"/>
+      <c r="O127" s="157"/>
+      <c r="P127" s="157"/>
+      <c r="Q127" s="157"/>
+      <c r="R127" s="157"/>
+      <c r="S127" s="157"/>
+      <c r="T127" s="157"/>
+      <c r="U127" s="157"/>
+      <c r="V127" s="157"/>
+      <c r="W127" s="157"/>
+      <c r="X127" s="157"/>
+      <c r="Y127" s="157"/>
     </row>
     <row r="128" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="122"/>
-      <c r="B128" s="122"/>
+      <c r="A128" s="156"/>
+      <c r="B128" s="156"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
@@ -11055,8 +11055,8 @@
       <c r="Y128" s="5"/>
     </row>
     <row r="129" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="122"/>
-      <c r="B129" s="122"/>
+      <c r="A129" s="156"/>
+      <c r="B129" s="156"/>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -11082,8 +11082,8 @@
       <c r="Y129" s="9"/>
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A130" s="116"/>
-      <c r="B130" s="116"/>
+      <c r="A130" s="110"/>
+      <c r="B130" s="110"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
@@ -11109,8 +11109,8 @@
       <c r="Y130" s="6"/>
     </row>
     <row r="131" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A131" s="116"/>
-      <c r="B131" s="116"/>
+      <c r="A131" s="110"/>
+      <c r="B131" s="110"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
       <c r="E131" s="6"/>
@@ -11136,8 +11136,8 @@
       <c r="Y131" s="6"/>
     </row>
     <row r="132" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A132" s="116"/>
-      <c r="B132" s="116"/>
+      <c r="A132" s="110"/>
+      <c r="B132" s="110"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
@@ -11163,8 +11163,8 @@
       <c r="Y132" s="6"/>
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A133" s="116"/>
-      <c r="B133" s="116"/>
+      <c r="A133" s="110"/>
+      <c r="B133" s="110"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
@@ -11244,35 +11244,35 @@
       <c r="Y135" s="6"/>
     </row>
     <row r="136" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="123"/>
-      <c r="B136" s="123"/>
-      <c r="C136" s="121"/>
-      <c r="D136" s="121"/>
-      <c r="E136" s="121"/>
-      <c r="F136" s="121"/>
-      <c r="G136" s="121"/>
-      <c r="H136" s="121"/>
-      <c r="I136" s="121"/>
-      <c r="J136" s="121"/>
-      <c r="K136" s="121"/>
-      <c r="L136" s="121"/>
-      <c r="M136" s="121"/>
-      <c r="N136" s="121"/>
-      <c r="O136" s="121"/>
-      <c r="P136" s="121"/>
-      <c r="Q136" s="121"/>
-      <c r="R136" s="121"/>
-      <c r="S136" s="121"/>
-      <c r="T136" s="121"/>
-      <c r="U136" s="121"/>
-      <c r="V136" s="121"/>
-      <c r="W136" s="121"/>
-      <c r="X136" s="121"/>
-      <c r="Y136" s="121"/>
+      <c r="A136" s="158"/>
+      <c r="B136" s="158"/>
+      <c r="C136" s="157"/>
+      <c r="D136" s="157"/>
+      <c r="E136" s="157"/>
+      <c r="F136" s="157"/>
+      <c r="G136" s="157"/>
+      <c r="H136" s="157"/>
+      <c r="I136" s="157"/>
+      <c r="J136" s="157"/>
+      <c r="K136" s="157"/>
+      <c r="L136" s="157"/>
+      <c r="M136" s="157"/>
+      <c r="N136" s="157"/>
+      <c r="O136" s="157"/>
+      <c r="P136" s="157"/>
+      <c r="Q136" s="157"/>
+      <c r="R136" s="157"/>
+      <c r="S136" s="157"/>
+      <c r="T136" s="157"/>
+      <c r="U136" s="157"/>
+      <c r="V136" s="157"/>
+      <c r="W136" s="157"/>
+      <c r="X136" s="157"/>
+      <c r="Y136" s="157"/>
     </row>
     <row r="137" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="122"/>
-      <c r="B137" s="122"/>
+      <c r="A137" s="156"/>
+      <c r="B137" s="156"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
@@ -11298,8 +11298,8 @@
       <c r="Y137" s="5"/>
     </row>
     <row r="138" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="122"/>
-      <c r="B138" s="122"/>
+      <c r="A138" s="156"/>
+      <c r="B138" s="156"/>
       <c r="C138" s="9"/>
       <c r="D138" s="9"/>
       <c r="E138" s="9"/>
@@ -11325,8 +11325,8 @@
       <c r="Y138" s="9"/>
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A139" s="116"/>
-      <c r="B139" s="116"/>
+      <c r="A139" s="110"/>
+      <c r="B139" s="110"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
@@ -11352,8 +11352,8 @@
       <c r="Y139" s="6"/>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A140" s="116"/>
-      <c r="B140" s="116"/>
+      <c r="A140" s="110"/>
+      <c r="B140" s="110"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
       <c r="E140" s="6"/>
@@ -11379,8 +11379,8 @@
       <c r="Y140" s="6"/>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A141" s="116"/>
-      <c r="B141" s="116"/>
+      <c r="A141" s="110"/>
+      <c r="B141" s="110"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
       <c r="E141" s="6"/>
@@ -11406,8 +11406,8 @@
       <c r="Y141" s="6"/>
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A142" s="116"/>
-      <c r="B142" s="116"/>
+      <c r="A142" s="110"/>
+      <c r="B142" s="110"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
       <c r="E142" s="6"/>
@@ -11487,35 +11487,35 @@
       <c r="Y144" s="6"/>
     </row>
     <row r="145" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="123"/>
-      <c r="B145" s="123"/>
-      <c r="C145" s="121"/>
-      <c r="D145" s="121"/>
-      <c r="E145" s="121"/>
-      <c r="F145" s="121"/>
-      <c r="G145" s="121"/>
-      <c r="H145" s="121"/>
-      <c r="I145" s="121"/>
-      <c r="J145" s="121"/>
-      <c r="K145" s="121"/>
-      <c r="L145" s="121"/>
-      <c r="M145" s="121"/>
-      <c r="N145" s="121"/>
-      <c r="O145" s="121"/>
-      <c r="P145" s="121"/>
-      <c r="Q145" s="121"/>
-      <c r="R145" s="121"/>
-      <c r="S145" s="121"/>
-      <c r="T145" s="121"/>
-      <c r="U145" s="121"/>
-      <c r="V145" s="121"/>
-      <c r="W145" s="121"/>
-      <c r="X145" s="121"/>
-      <c r="Y145" s="121"/>
+      <c r="A145" s="158"/>
+      <c r="B145" s="158"/>
+      <c r="C145" s="157"/>
+      <c r="D145" s="157"/>
+      <c r="E145" s="157"/>
+      <c r="F145" s="157"/>
+      <c r="G145" s="157"/>
+      <c r="H145" s="157"/>
+      <c r="I145" s="157"/>
+      <c r="J145" s="157"/>
+      <c r="K145" s="157"/>
+      <c r="L145" s="157"/>
+      <c r="M145" s="157"/>
+      <c r="N145" s="157"/>
+      <c r="O145" s="157"/>
+      <c r="P145" s="157"/>
+      <c r="Q145" s="157"/>
+      <c r="R145" s="157"/>
+      <c r="S145" s="157"/>
+      <c r="T145" s="157"/>
+      <c r="U145" s="157"/>
+      <c r="V145" s="157"/>
+      <c r="W145" s="157"/>
+      <c r="X145" s="157"/>
+      <c r="Y145" s="157"/>
     </row>
     <row r="146" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="122"/>
-      <c r="B146" s="122"/>
+      <c r="A146" s="156"/>
+      <c r="B146" s="156"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
@@ -11541,8 +11541,8 @@
       <c r="Y146" s="5"/>
     </row>
     <row r="147" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="122"/>
-      <c r="B147" s="122"/>
+      <c r="A147" s="156"/>
+      <c r="B147" s="156"/>
       <c r="C147" s="9"/>
       <c r="D147" s="9"/>
       <c r="E147" s="9"/>
@@ -11568,8 +11568,8 @@
       <c r="Y147" s="9"/>
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A148" s="116"/>
-      <c r="B148" s="116"/>
+      <c r="A148" s="110"/>
+      <c r="B148" s="110"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
@@ -11595,8 +11595,8 @@
       <c r="Y148" s="6"/>
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A149" s="116"/>
-      <c r="B149" s="116"/>
+      <c r="A149" s="110"/>
+      <c r="B149" s="110"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
@@ -11622,8 +11622,8 @@
       <c r="Y149" s="6"/>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A150" s="116"/>
-      <c r="B150" s="116"/>
+      <c r="A150" s="110"/>
+      <c r="B150" s="110"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
@@ -11649,8 +11649,8 @@
       <c r="Y150" s="6"/>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A151" s="116"/>
-      <c r="B151" s="116"/>
+      <c r="A151" s="110"/>
+      <c r="B151" s="110"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
@@ -11730,35 +11730,35 @@
       <c r="Y153" s="4"/>
     </row>
     <row r="154" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="123"/>
-      <c r="B154" s="123"/>
-      <c r="C154" s="121"/>
-      <c r="D154" s="121"/>
-      <c r="E154" s="121"/>
-      <c r="F154" s="121"/>
-      <c r="G154" s="121"/>
-      <c r="H154" s="121"/>
-      <c r="I154" s="121"/>
-      <c r="J154" s="121"/>
-      <c r="K154" s="121"/>
-      <c r="L154" s="121"/>
-      <c r="M154" s="121"/>
-      <c r="N154" s="121"/>
-      <c r="O154" s="121"/>
-      <c r="P154" s="121"/>
-      <c r="Q154" s="121"/>
-      <c r="R154" s="121"/>
-      <c r="S154" s="121"/>
-      <c r="T154" s="121"/>
-      <c r="U154" s="121"/>
-      <c r="V154" s="121"/>
-      <c r="W154" s="121"/>
-      <c r="X154" s="121"/>
-      <c r="Y154" s="121"/>
+      <c r="A154" s="158"/>
+      <c r="B154" s="158"/>
+      <c r="C154" s="157"/>
+      <c r="D154" s="157"/>
+      <c r="E154" s="157"/>
+      <c r="F154" s="157"/>
+      <c r="G154" s="157"/>
+      <c r="H154" s="157"/>
+      <c r="I154" s="157"/>
+      <c r="J154" s="157"/>
+      <c r="K154" s="157"/>
+      <c r="L154" s="157"/>
+      <c r="M154" s="157"/>
+      <c r="N154" s="157"/>
+      <c r="O154" s="157"/>
+      <c r="P154" s="157"/>
+      <c r="Q154" s="157"/>
+      <c r="R154" s="157"/>
+      <c r="S154" s="157"/>
+      <c r="T154" s="157"/>
+      <c r="U154" s="157"/>
+      <c r="V154" s="157"/>
+      <c r="W154" s="157"/>
+      <c r="X154" s="157"/>
+      <c r="Y154" s="157"/>
     </row>
     <row r="155" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="122"/>
-      <c r="B155" s="122"/>
+      <c r="A155" s="156"/>
+      <c r="B155" s="156"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
@@ -11784,8 +11784,8 @@
       <c r="Y155" s="5"/>
     </row>
     <row r="156" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="122"/>
-      <c r="B156" s="122"/>
+      <c r="A156" s="156"/>
+      <c r="B156" s="156"/>
       <c r="C156" s="9"/>
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
@@ -11811,8 +11811,8 @@
       <c r="Y156" s="9"/>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A157" s="116"/>
-      <c r="B157" s="116"/>
+      <c r="A157" s="110"/>
+      <c r="B157" s="110"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="E157" s="6"/>
@@ -11838,8 +11838,8 @@
       <c r="Y157" s="6"/>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A158" s="116"/>
-      <c r="B158" s="116"/>
+      <c r="A158" s="110"/>
+      <c r="B158" s="110"/>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
@@ -11865,8 +11865,8 @@
       <c r="Y158" s="6"/>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A159" s="116"/>
-      <c r="B159" s="116"/>
+      <c r="A159" s="110"/>
+      <c r="B159" s="110"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="6"/>
@@ -11892,8 +11892,8 @@
       <c r="Y159" s="6"/>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A160" s="116"/>
-      <c r="B160" s="116"/>
+      <c r="A160" s="110"/>
+      <c r="B160" s="110"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="E160" s="6"/>
@@ -11973,35 +11973,35 @@
       <c r="Y162" s="6"/>
     </row>
     <row r="163" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="123"/>
-      <c r="B163" s="123"/>
-      <c r="C163" s="121"/>
-      <c r="D163" s="121"/>
-      <c r="E163" s="121"/>
-      <c r="F163" s="121"/>
-      <c r="G163" s="121"/>
-      <c r="H163" s="121"/>
-      <c r="I163" s="121"/>
-      <c r="J163" s="121"/>
-      <c r="K163" s="121"/>
-      <c r="L163" s="121"/>
-      <c r="M163" s="121"/>
-      <c r="N163" s="121"/>
-      <c r="O163" s="121"/>
-      <c r="P163" s="121"/>
-      <c r="Q163" s="121"/>
-      <c r="R163" s="121"/>
-      <c r="S163" s="121"/>
-      <c r="T163" s="121"/>
-      <c r="U163" s="121"/>
-      <c r="V163" s="121"/>
-      <c r="W163" s="121"/>
-      <c r="X163" s="121"/>
-      <c r="Y163" s="121"/>
+      <c r="A163" s="158"/>
+      <c r="B163" s="158"/>
+      <c r="C163" s="157"/>
+      <c r="D163" s="157"/>
+      <c r="E163" s="157"/>
+      <c r="F163" s="157"/>
+      <c r="G163" s="157"/>
+      <c r="H163" s="157"/>
+      <c r="I163" s="157"/>
+      <c r="J163" s="157"/>
+      <c r="K163" s="157"/>
+      <c r="L163" s="157"/>
+      <c r="M163" s="157"/>
+      <c r="N163" s="157"/>
+      <c r="O163" s="157"/>
+      <c r="P163" s="157"/>
+      <c r="Q163" s="157"/>
+      <c r="R163" s="157"/>
+      <c r="S163" s="157"/>
+      <c r="T163" s="157"/>
+      <c r="U163" s="157"/>
+      <c r="V163" s="157"/>
+      <c r="W163" s="157"/>
+      <c r="X163" s="157"/>
+      <c r="Y163" s="157"/>
     </row>
     <row r="164" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="122"/>
-      <c r="B164" s="122"/>
+      <c r="A164" s="156"/>
+      <c r="B164" s="156"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
@@ -12027,8 +12027,8 @@
       <c r="Y164" s="5"/>
     </row>
     <row r="165" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="122"/>
-      <c r="B165" s="122"/>
+      <c r="A165" s="156"/>
+      <c r="B165" s="156"/>
       <c r="C165" s="9"/>
       <c r="D165" s="9"/>
       <c r="E165" s="9"/>
@@ -12054,8 +12054,8 @@
       <c r="Y165" s="9"/>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A166" s="116"/>
-      <c r="B166" s="116"/>
+      <c r="A166" s="110"/>
+      <c r="B166" s="110"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="E166" s="6"/>
@@ -12081,8 +12081,8 @@
       <c r="Y166" s="6"/>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A167" s="116"/>
-      <c r="B167" s="116"/>
+      <c r="A167" s="110"/>
+      <c r="B167" s="110"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="E167" s="6"/>
@@ -12108,8 +12108,8 @@
       <c r="Y167" s="6"/>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A168" s="116"/>
-      <c r="B168" s="116"/>
+      <c r="A168" s="110"/>
+      <c r="B168" s="110"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="E168" s="6"/>
@@ -12135,8 +12135,8 @@
       <c r="Y168" s="6"/>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A169" s="116"/>
-      <c r="B169" s="116"/>
+      <c r="A169" s="110"/>
+      <c r="B169" s="110"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="E169" s="6"/>
@@ -12216,35 +12216,35 @@
       <c r="Y171" s="6"/>
     </row>
     <row r="172" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="123"/>
-      <c r="B172" s="123"/>
-      <c r="C172" s="121"/>
-      <c r="D172" s="121"/>
-      <c r="E172" s="121"/>
-      <c r="F172" s="121"/>
-      <c r="G172" s="121"/>
-      <c r="H172" s="121"/>
-      <c r="I172" s="121"/>
-      <c r="J172" s="121"/>
-      <c r="K172" s="121"/>
-      <c r="L172" s="121"/>
-      <c r="M172" s="121"/>
-      <c r="N172" s="121"/>
-      <c r="O172" s="121"/>
-      <c r="P172" s="121"/>
-      <c r="Q172" s="121"/>
-      <c r="R172" s="121"/>
-      <c r="S172" s="121"/>
-      <c r="T172" s="121"/>
-      <c r="U172" s="121"/>
-      <c r="V172" s="121"/>
-      <c r="W172" s="121"/>
-      <c r="X172" s="121"/>
-      <c r="Y172" s="121"/>
+      <c r="A172" s="158"/>
+      <c r="B172" s="158"/>
+      <c r="C172" s="157"/>
+      <c r="D172" s="157"/>
+      <c r="E172" s="157"/>
+      <c r="F172" s="157"/>
+      <c r="G172" s="157"/>
+      <c r="H172" s="157"/>
+      <c r="I172" s="157"/>
+      <c r="J172" s="157"/>
+      <c r="K172" s="157"/>
+      <c r="L172" s="157"/>
+      <c r="M172" s="157"/>
+      <c r="N172" s="157"/>
+      <c r="O172" s="157"/>
+      <c r="P172" s="157"/>
+      <c r="Q172" s="157"/>
+      <c r="R172" s="157"/>
+      <c r="S172" s="157"/>
+      <c r="T172" s="157"/>
+      <c r="U172" s="157"/>
+      <c r="V172" s="157"/>
+      <c r="W172" s="157"/>
+      <c r="X172" s="157"/>
+      <c r="Y172" s="157"/>
     </row>
     <row r="173" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="122"/>
-      <c r="B173" s="122"/>
+      <c r="A173" s="156"/>
+      <c r="B173" s="156"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
@@ -12270,8 +12270,8 @@
       <c r="Y173" s="5"/>
     </row>
     <row r="174" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="122"/>
-      <c r="B174" s="122"/>
+      <c r="A174" s="156"/>
+      <c r="B174" s="156"/>
       <c r="C174" s="9"/>
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
@@ -12297,8 +12297,8 @@
       <c r="Y174" s="9"/>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A175" s="116"/>
-      <c r="B175" s="116"/>
+      <c r="A175" s="110"/>
+      <c r="B175" s="110"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
@@ -12324,8 +12324,8 @@
       <c r="Y175" s="6"/>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A176" s="116"/>
-      <c r="B176" s="116"/>
+      <c r="A176" s="110"/>
+      <c r="B176" s="110"/>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="E176" s="6"/>
@@ -12351,8 +12351,8 @@
       <c r="Y176" s="6"/>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A177" s="116"/>
-      <c r="B177" s="116"/>
+      <c r="A177" s="110"/>
+      <c r="B177" s="110"/>
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="E177" s="6"/>
@@ -12378,8 +12378,8 @@
       <c r="Y177" s="6"/>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A178" s="116"/>
-      <c r="B178" s="116"/>
+      <c r="A178" s="110"/>
+      <c r="B178" s="110"/>
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="E178" s="6"/>
@@ -12459,35 +12459,35 @@
       <c r="Y180" s="6"/>
     </row>
     <row r="181" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="123"/>
-      <c r="B181" s="123"/>
-      <c r="C181" s="121"/>
-      <c r="D181" s="121"/>
-      <c r="E181" s="121"/>
-      <c r="F181" s="121"/>
-      <c r="G181" s="121"/>
-      <c r="H181" s="121"/>
-      <c r="I181" s="121"/>
-      <c r="J181" s="121"/>
-      <c r="K181" s="121"/>
-      <c r="L181" s="121"/>
-      <c r="M181" s="121"/>
-      <c r="N181" s="121"/>
-      <c r="O181" s="121"/>
-      <c r="P181" s="121"/>
-      <c r="Q181" s="121"/>
-      <c r="R181" s="121"/>
-      <c r="S181" s="121"/>
-      <c r="T181" s="121"/>
-      <c r="U181" s="121"/>
-      <c r="V181" s="121"/>
-      <c r="W181" s="121"/>
-      <c r="X181" s="121"/>
-      <c r="Y181" s="121"/>
+      <c r="A181" s="158"/>
+      <c r="B181" s="158"/>
+      <c r="C181" s="157"/>
+      <c r="D181" s="157"/>
+      <c r="E181" s="157"/>
+      <c r="F181" s="157"/>
+      <c r="G181" s="157"/>
+      <c r="H181" s="157"/>
+      <c r="I181" s="157"/>
+      <c r="J181" s="157"/>
+      <c r="K181" s="157"/>
+      <c r="L181" s="157"/>
+      <c r="M181" s="157"/>
+      <c r="N181" s="157"/>
+      <c r="O181" s="157"/>
+      <c r="P181" s="157"/>
+      <c r="Q181" s="157"/>
+      <c r="R181" s="157"/>
+      <c r="S181" s="157"/>
+      <c r="T181" s="157"/>
+      <c r="U181" s="157"/>
+      <c r="V181" s="157"/>
+      <c r="W181" s="157"/>
+      <c r="X181" s="157"/>
+      <c r="Y181" s="157"/>
     </row>
     <row r="182" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="122"/>
-      <c r="B182" s="122"/>
+      <c r="A182" s="156"/>
+      <c r="B182" s="156"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
       <c r="E182" s="5"/>
@@ -12513,8 +12513,8 @@
       <c r="Y182" s="5"/>
     </row>
     <row r="183" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="122"/>
-      <c r="B183" s="122"/>
+      <c r="A183" s="156"/>
+      <c r="B183" s="156"/>
       <c r="C183" s="9"/>
       <c r="D183" s="9"/>
       <c r="E183" s="9"/>
@@ -12540,8 +12540,8 @@
       <c r="Y183" s="9"/>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A184" s="116"/>
-      <c r="B184" s="116"/>
+      <c r="A184" s="110"/>
+      <c r="B184" s="110"/>
       <c r="C184" s="6"/>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
@@ -12567,8 +12567,8 @@
       <c r="Y184" s="6"/>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A185" s="116"/>
-      <c r="B185" s="116"/>
+      <c r="A185" s="110"/>
+      <c r="B185" s="110"/>
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
@@ -12594,8 +12594,8 @@
       <c r="Y185" s="6"/>
     </row>
     <row r="186" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A186" s="116"/>
-      <c r="B186" s="116"/>
+      <c r="A186" s="110"/>
+      <c r="B186" s="110"/>
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="E186" s="6"/>
@@ -12621,8 +12621,8 @@
       <c r="Y186" s="6"/>
     </row>
     <row r="187" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A187" s="116"/>
-      <c r="B187" s="116"/>
+      <c r="A187" s="110"/>
+      <c r="B187" s="110"/>
       <c r="C187" s="6"/>
       <c r="D187" s="6"/>
       <c r="E187" s="6"/>
@@ -43834,6 +43834,158 @@
     </row>
   </sheetData>
   <mergeCells count="176">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="F41:M41"/>
+    <mergeCell ref="F43:M43"/>
+    <mergeCell ref="F45:M45"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="F33:M33"/>
+    <mergeCell ref="O29:W36"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="F29:M29"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="F31:M31"/>
+    <mergeCell ref="F35:M35"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="F39:M39"/>
+    <mergeCell ref="A25:S26"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="A4:W4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C163:Y163"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="C108:Y108"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="C99:Y99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="C89:Y89"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="C117:Y117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="C154:Y154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="C145:Y145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="C136:Y136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="C127:Y127"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="C181:Y181"/>
+    <mergeCell ref="C172:Y172"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="C80:Y80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C71:Y71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C60:Y60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="Q13:W13"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="I13:L13"/>
     <mergeCell ref="A3:W3"/>
     <mergeCell ref="M13:P13"/>
     <mergeCell ref="A34:B34"/>
@@ -43858,165 +44010,14 @@
     <mergeCell ref="T10:W10"/>
     <mergeCell ref="T11:W11"/>
     <mergeCell ref="T9:W9"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="Q13:W13"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C71:Y71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C60:Y60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C80:Y80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="C181:Y181"/>
-    <mergeCell ref="C172:Y172"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="C154:Y154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="C145:Y145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="C136:Y136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="C127:Y127"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C163:Y163"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="C108:Y108"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="C99:Y99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="C89:Y89"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="C117:Y117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A43:E43"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="F41:M41"/>
-    <mergeCell ref="F43:M43"/>
-    <mergeCell ref="F45:M45"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="F33:M33"/>
-    <mergeCell ref="O29:W36"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="F29:M29"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="F31:M31"/>
-    <mergeCell ref="F35:M35"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="F39:M39"/>
-    <mergeCell ref="A25:S26"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="A4:W4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.98425196850393704" right="0.51181102362204722" top="0.74803149606299213" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.51181102362204722"/>
   <pageSetup scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"-,Bold"&amp;16Xpert TB Proficiency Test Result Form</oddHeader>
-    <oddFooter>&amp;LILB-500-F29C&amp;CIssuing Authority: David Turgeon</oddFooter>
+    <oddFooter>&amp;LILB-500-F29C&amp;C&amp;P of &amp;N
+Issuing Authority: David Turgeon</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="26" max="16383" man="1"/>
@@ -44080,6 +44081,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001821B2EC25D39140BA1AC3A0F93B26A5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b58428e78da37c37572897deebd74128">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -44128,15 +44138,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
   <ds:schemaRefs>
@@ -44152,6 +44153,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EECD6A4-5CAC-4EB2-BF99-66BCF0600A47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44164,12 +44173,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix(Trello-45): fixes to result submission form requested by Mariela
</commit_message>
<xml_diff>
--- a/public/templates/ept_tb_submission_form_1.3.xlsx
+++ b/public/templates/ept_tb_submission_form_1.3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brich\projects\SystemOne\ept\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ept\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD9D269-7FE7-4956-AA2E-D72C294364FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CC98B0-CF7C-4E33-B544-2B0AA3B5522E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,56 +186,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This form is for your site's performance evaluation records only.  All results must be submitted in ePT at </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>http://ept.systemone.id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> using your username and password above. </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Submission Due Date: </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ATTESTATION</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-We the undersigned, recognizing that some special handling may be required due to the nature of Performance Evaluation (PE) materials, have as closely as is practical, performed the analyses on these specimens in the same manner as regular patient specimens.  We confirm that results were not shared, nor PE specimens referred or tested, outside of our facility. 
-Laboratory Manager (or Designee) ____________________  Date:______
-Testing Personnel   _______________________      Date:______________                                                                                                                                                Testing Personnel   _______________________      Date:______________
-</t>
-    </r>
   </si>
   <si>
     <t>Assay</t>
@@ -288,13 +239,63 @@
   <si>
     <t xml:space="preserve">Proficiency Test Panel ID:  </t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ATTESTATION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+We the undersigned, recognizing that some special handling may be required due to the nature of Proficiency Test (PT) materials, have as closely as is practical, performed the analyses on these specimens in the same manner as regular patient specimens.  We confirm that results were not shared, nor PT specimens referred or tested, outside of our facility. 
+Laboratory Manager (or Designee) ____________________  Date:______
+Testing Personnel   _______________________      Date:______________                                                                                                                                                Testing Personnel   _______________________      Date:______________
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This form is for your site's performance evaluation records only.  All results must be submitted in ePT at </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://ept.systemone.id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using your username and password above. </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -1281,11 +1282,101 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,31 +1387,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1395,77 +1465,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7442,14 +7443,14 @@
   </sheetPr>
   <dimension ref="A1:Y1342"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="W1" sqref="A1:W47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScale="120" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="8" width="3.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
@@ -7464,33 +7465,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="160" t="s">
-        <v>59</v>
+      <c r="A1" s="105" t="s">
+        <v>57</v>
       </c>
-      <c r="B1" s="160"/>
-      <c r="C1" s="160"/>
-      <c r="D1" s="160"/>
-      <c r="E1" s="160"/>
-      <c r="F1" s="160"/>
-      <c r="G1" s="160"/>
-      <c r="H1" s="160"/>
-      <c r="I1" s="160"/>
-      <c r="J1" s="160"/>
-      <c r="K1" s="161" t="s">
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="105"/>
+      <c r="G1" s="105"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="166" t="s">
-        <v>45</v>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="118" t="s">
+        <v>44</v>
       </c>
-      <c r="T1" s="166"/>
-      <c r="U1" s="166"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
       <c r="V1" s="99"/>
       <c r="W1" s="99"/>
       <c r="X1" s="76"/>
@@ -7524,91 +7525,91 @@
       <c r="Y2" s="77"/>
     </row>
     <row r="3" spans="1:25" s="1" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="106"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="106"/>
-      <c r="O3" s="106"/>
-      <c r="P3" s="106"/>
-      <c r="Q3" s="106"/>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="119"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="119"/>
+      <c r="G3" s="119"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="119"/>
+      <c r="J3" s="119"/>
+      <c r="K3" s="119"/>
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="119"/>
+      <c r="S3" s="119"/>
+      <c r="T3" s="119"/>
+      <c r="U3" s="119"/>
+      <c r="V3" s="119"/>
+      <c r="W3" s="119"/>
       <c r="X3" s="25"/>
       <c r="Y3" s="76"/>
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" ht="8.4499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106"/>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="106"/>
+      <c r="A4" s="119"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
+      <c r="J4" s="119"/>
+      <c r="K4" s="119"/>
+      <c r="L4" s="119"/>
+      <c r="M4" s="119"/>
+      <c r="N4" s="119"/>
+      <c r="O4" s="119"/>
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119"/>
+      <c r="R4" s="119"/>
+      <c r="S4" s="119"/>
+      <c r="T4" s="119"/>
+      <c r="U4" s="119"/>
+      <c r="V4" s="119"/>
+      <c r="W4" s="119"/>
       <c r="X4" s="27"/>
       <c r="Y4" s="76"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="144"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="117"/>
-      <c r="K5" s="117"/>
-      <c r="L5" s="117"/>
+      <c r="B5" s="125"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
       <c r="M5" s="104"/>
       <c r="N5" s="22"/>
-      <c r="O5" s="111" t="s">
+      <c r="O5" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="112"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="111" t="s">
+      <c r="P5" s="109"/>
+      <c r="Q5" s="109"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="113"/>
+      <c r="T5" s="109"/>
+      <c r="U5" s="109"/>
+      <c r="V5" s="109"/>
+      <c r="W5" s="110"/>
       <c r="X5" s="78"/>
       <c r="Y5" s="79"/>
     </row>
@@ -7627,33 +7628,33 @@
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
-      <c r="O6" s="118"/>
-      <c r="P6" s="114"/>
-      <c r="Q6" s="114"/>
-      <c r="R6" s="115"/>
-      <c r="S6" s="119"/>
-      <c r="T6" s="120"/>
-      <c r="U6" s="120"/>
-      <c r="V6" s="120"/>
-      <c r="W6" s="121"/>
+      <c r="O6" s="111"/>
+      <c r="P6" s="112"/>
+      <c r="Q6" s="112"/>
+      <c r="R6" s="113"/>
+      <c r="S6" s="142"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="144"/>
       <c r="X6" s="78"/>
       <c r="Y6" s="79"/>
     </row>
     <row r="7" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="108" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="144"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="117"/>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
       <c r="M7" s="103"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
@@ -7683,50 +7684,50 @@
       <c r="L8" s="16"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="122" t="s">
+      <c r="O8" s="145" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="123"/>
-      <c r="Q8" s="123"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="124"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="132"/>
-      <c r="W8" s="133"/>
+      <c r="P8" s="146"/>
+      <c r="Q8" s="146"/>
+      <c r="R8" s="146"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="154"/>
+      <c r="U8" s="155"/>
+      <c r="V8" s="155"/>
+      <c r="W8" s="156"/>
       <c r="X8" s="75"/>
       <c r="Y8" s="25"/>
     </row>
     <row r="9" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111" t="s">
+      <c r="A9" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="116"/>
-      <c r="D9" s="117"/>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="117"/>
-      <c r="K9" s="117"/>
-      <c r="L9" s="117"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="141"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="141"/>
+      <c r="K9" s="141"/>
+      <c r="L9" s="141"/>
       <c r="M9" s="103"/>
       <c r="N9" s="22"/>
-      <c r="O9" s="125" t="s">
-        <v>47</v>
+      <c r="O9" s="148" t="s">
+        <v>45</v>
       </c>
-      <c r="P9" s="126"/>
-      <c r="Q9" s="126"/>
-      <c r="R9" s="126"/>
-      <c r="S9" s="127"/>
-      <c r="T9" s="140" t="s">
-        <v>55</v>
+      <c r="P9" s="149"/>
+      <c r="Q9" s="149"/>
+      <c r="R9" s="149"/>
+      <c r="S9" s="150"/>
+      <c r="T9" s="163" t="s">
+        <v>53</v>
       </c>
-      <c r="U9" s="141"/>
-      <c r="V9" s="141"/>
-      <c r="W9" s="142"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="164"/>
+      <c r="W9" s="165"/>
       <c r="X9" s="75"/>
       <c r="Y9" s="12"/>
     </row>
@@ -7745,48 +7746,48 @@
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
-      <c r="O10" s="125" t="s">
-        <v>56</v>
+      <c r="O10" s="148" t="s">
+        <v>54</v>
       </c>
-      <c r="P10" s="126"/>
-      <c r="Q10" s="126"/>
-      <c r="R10" s="126"/>
-      <c r="S10" s="127"/>
-      <c r="T10" s="134"/>
-      <c r="U10" s="135"/>
-      <c r="V10" s="135"/>
-      <c r="W10" s="136"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="150"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="158"/>
+      <c r="V10" s="158"/>
+      <c r="W10" s="159"/>
       <c r="X10" s="22"/>
       <c r="Y10" s="5"/>
     </row>
     <row r="11" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="117"/>
-      <c r="F11" s="117"/>
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="117"/>
-      <c r="J11" s="117"/>
-      <c r="K11" s="117"/>
-      <c r="L11" s="117"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="141"/>
+      <c r="L11" s="141"/>
       <c r="M11" s="103"/>
       <c r="N11" s="22"/>
-      <c r="O11" s="128" t="s">
-        <v>57</v>
+      <c r="O11" s="151" t="s">
+        <v>55</v>
       </c>
-      <c r="P11" s="129"/>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
-      <c r="S11" s="130"/>
-      <c r="T11" s="137"/>
-      <c r="U11" s="138"/>
-      <c r="V11" s="138"/>
-      <c r="W11" s="139"/>
+      <c r="P11" s="152"/>
+      <c r="Q11" s="152"/>
+      <c r="R11" s="152"/>
+      <c r="S11" s="153"/>
+      <c r="T11" s="160"/>
+      <c r="U11" s="161"/>
+      <c r="V11" s="161"/>
+      <c r="W11" s="162"/>
       <c r="X11" s="22"/>
       <c r="Y11" s="13"/>
     </row>
@@ -7818,37 +7819,37 @@
       <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:25" ht="31.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="148"/>
-      <c r="B13" s="149"/>
-      <c r="C13" s="145" t="s">
+      <c r="A13" s="129"/>
+      <c r="B13" s="130"/>
+      <c r="C13" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="146"/>
-      <c r="E13" s="146"/>
-      <c r="F13" s="146"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="154" t="s">
+      <c r="D13" s="127"/>
+      <c r="E13" s="127"/>
+      <c r="F13" s="127"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="128"/>
+      <c r="I13" s="135" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="155"/>
-      <c r="K13" s="155"/>
-      <c r="L13" s="155"/>
-      <c r="M13" s="107" t="s">
+      <c r="J13" s="136"/>
+      <c r="K13" s="136"/>
+      <c r="L13" s="136"/>
+      <c r="M13" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="N13" s="108"/>
-      <c r="O13" s="108"/>
-      <c r="P13" s="109"/>
-      <c r="Q13" s="150" t="s">
+      <c r="N13" s="138"/>
+      <c r="O13" s="138"/>
+      <c r="P13" s="139"/>
+      <c r="Q13" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="R13" s="151"/>
-      <c r="S13" s="151"/>
-      <c r="T13" s="151"/>
-      <c r="U13" s="151"/>
-      <c r="V13" s="151"/>
-      <c r="W13" s="152"/>
+      <c r="R13" s="132"/>
+      <c r="S13" s="132"/>
+      <c r="T13" s="132"/>
+      <c r="U13" s="132"/>
+      <c r="V13" s="132"/>
+      <c r="W13" s="133"/>
       <c r="X13" s="79"/>
       <c r="Y13" s="25"/>
     </row>
@@ -7863,7 +7864,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="44" t="s">
         <v>10</v>
@@ -7902,22 +7903,22 @@
         <v>19</v>
       </c>
       <c r="Q14" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="S14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="T14" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="S14" s="21" t="s">
+      <c r="U14" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="T14" s="21" t="s">
+      <c r="V14" s="30" t="s">
         <v>52</v>
-      </c>
-      <c r="U14" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="V14" s="30" t="s">
-        <v>54</v>
       </c>
       <c r="W14" s="98" t="s">
         <v>30</v>
@@ -7929,7 +7930,7 @@
       <c r="A15" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="105">
+      <c r="B15" s="166">
         <v>43235</v>
       </c>
       <c r="C15" s="46"/>
@@ -8133,10 +8134,10 @@
       <c r="Y21" s="12"/>
     </row>
     <row r="22" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="153" t="s">
+      <c r="A22" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="153"/>
+      <c r="B22" s="134"/>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
       <c r="E22" s="26"/>
@@ -8216,27 +8217,27 @@
       <c r="Y24" s="12"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25" s="164" t="s">
-        <v>44</v>
+      <c r="A25" s="116" t="s">
+        <v>59</v>
       </c>
-      <c r="B25" s="164"/>
-      <c r="C25" s="164"/>
-      <c r="D25" s="164"/>
-      <c r="E25" s="164"/>
-      <c r="F25" s="164"/>
-      <c r="G25" s="164"/>
-      <c r="H25" s="164"/>
-      <c r="I25" s="164"/>
-      <c r="J25" s="164"/>
-      <c r="K25" s="164"/>
-      <c r="L25" s="164"/>
-      <c r="M25" s="164"/>
-      <c r="N25" s="164"/>
-      <c r="O25" s="164"/>
-      <c r="P25" s="164"/>
-      <c r="Q25" s="164"/>
-      <c r="R25" s="164"/>
-      <c r="S25" s="164"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="116"/>
+      <c r="J25" s="116"/>
+      <c r="K25" s="116"/>
+      <c r="L25" s="116"/>
+      <c r="M25" s="116"/>
+      <c r="N25" s="116"/>
+      <c r="O25" s="116"/>
+      <c r="P25" s="116"/>
+      <c r="Q25" s="116"/>
+      <c r="R25" s="116"/>
+      <c r="S25" s="116"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
@@ -8245,25 +8246,25 @@
       <c r="Y25" s="3"/>
     </row>
     <row r="26" spans="1:25" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="165"/>
-      <c r="B26" s="165"/>
-      <c r="C26" s="165"/>
-      <c r="D26" s="165"/>
-      <c r="E26" s="165"/>
-      <c r="F26" s="165"/>
-      <c r="G26" s="165"/>
-      <c r="H26" s="165"/>
-      <c r="I26" s="165"/>
-      <c r="J26" s="165"/>
-      <c r="K26" s="165"/>
-      <c r="L26" s="165"/>
-      <c r="M26" s="165"/>
-      <c r="N26" s="165"/>
-      <c r="O26" s="165"/>
-      <c r="P26" s="165"/>
-      <c r="Q26" s="165"/>
-      <c r="R26" s="165"/>
-      <c r="S26" s="165"/>
+      <c r="A26" s="117"/>
+      <c r="B26" s="117"/>
+      <c r="C26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="117"/>
+      <c r="F26" s="117"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="117"/>
+      <c r="K26" s="117"/>
+      <c r="L26" s="117"/>
+      <c r="M26" s="117"/>
+      <c r="N26" s="117"/>
+      <c r="O26" s="117"/>
+      <c r="P26" s="117"/>
+      <c r="Q26" s="117"/>
+      <c r="R26" s="117"/>
+      <c r="S26" s="117"/>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="7"/>
@@ -8301,8 +8302,8 @@
       <c r="Y27" s="6"/>
     </row>
     <row r="28" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="110"/>
-      <c r="B28" s="110"/>
+      <c r="A28" s="115"/>
+      <c r="B28" s="115"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -8328,33 +8329,33 @@
       <c r="Y28" s="7"/>
     </row>
     <row r="29" spans="1:25" s="1" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="111" t="s">
+      <c r="A29" s="108" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="109"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="112"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
+      <c r="K29" s="112"/>
+      <c r="L29" s="112"/>
+      <c r="M29" s="113"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="112"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="114"/>
-      <c r="H29" s="114"/>
-      <c r="I29" s="114"/>
-      <c r="J29" s="114"/>
-      <c r="K29" s="114"/>
-      <c r="L29" s="114"/>
-      <c r="M29" s="115"/>
-      <c r="N29" s="22"/>
-      <c r="O29" s="163" t="s">
-        <v>46</v>
-      </c>
-      <c r="P29" s="163"/>
-      <c r="Q29" s="163"/>
-      <c r="R29" s="163"/>
-      <c r="S29" s="163"/>
-      <c r="T29" s="163"/>
-      <c r="U29" s="163"/>
-      <c r="V29" s="163"/>
-      <c r="W29" s="163"/>
+      <c r="P29" s="114"/>
+      <c r="Q29" s="114"/>
+      <c r="R29" s="114"/>
+      <c r="S29" s="114"/>
+      <c r="T29" s="114"/>
+      <c r="U29" s="114"/>
+      <c r="V29" s="114"/>
+      <c r="W29" s="114"/>
       <c r="X29" s="78"/>
       <c r="Y29" s="79"/>
     </row>
@@ -8373,44 +8374,44 @@
       <c r="L30" s="23"/>
       <c r="M30" s="23"/>
       <c r="N30" s="23"/>
-      <c r="O30" s="163"/>
-      <c r="P30" s="163"/>
-      <c r="Q30" s="163"/>
-      <c r="R30" s="163"/>
-      <c r="S30" s="163"/>
-      <c r="T30" s="163"/>
-      <c r="U30" s="163"/>
-      <c r="V30" s="163"/>
-      <c r="W30" s="163"/>
+      <c r="O30" s="114"/>
+      <c r="P30" s="114"/>
+      <c r="Q30" s="114"/>
+      <c r="R30" s="114"/>
+      <c r="S30" s="114"/>
+      <c r="T30" s="114"/>
+      <c r="U30" s="114"/>
+      <c r="V30" s="114"/>
+      <c r="W30" s="114"/>
       <c r="X30" s="78"/>
       <c r="Y30" s="79"/>
     </row>
     <row r="31" spans="1:25" s="1" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111" t="s">
+      <c r="A31" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="112"/>
-      <c r="C31" s="112"/>
-      <c r="D31" s="112"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="114"/>
-      <c r="H31" s="114"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="114"/>
-      <c r="K31" s="114"/>
-      <c r="L31" s="114"/>
-      <c r="M31" s="115"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="112"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="113"/>
       <c r="N31" s="22"/>
-      <c r="O31" s="163"/>
-      <c r="P31" s="163"/>
-      <c r="Q31" s="163"/>
-      <c r="R31" s="163"/>
-      <c r="S31" s="163"/>
-      <c r="T31" s="163"/>
-      <c r="U31" s="163"/>
-      <c r="V31" s="163"/>
-      <c r="W31" s="163"/>
+      <c r="O31" s="114"/>
+      <c r="P31" s="114"/>
+      <c r="Q31" s="114"/>
+      <c r="R31" s="114"/>
+      <c r="S31" s="114"/>
+      <c r="T31" s="114"/>
+      <c r="U31" s="114"/>
+      <c r="V31" s="114"/>
+      <c r="W31" s="114"/>
       <c r="X31" s="24"/>
       <c r="Y31" s="12"/>
     </row>
@@ -8429,50 +8430,50 @@
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
-      <c r="O32" s="163"/>
-      <c r="P32" s="163"/>
-      <c r="Q32" s="163"/>
-      <c r="R32" s="163"/>
-      <c r="S32" s="163"/>
-      <c r="T32" s="163"/>
-      <c r="U32" s="163"/>
-      <c r="V32" s="163"/>
-      <c r="W32" s="163"/>
+      <c r="O32" s="114"/>
+      <c r="P32" s="114"/>
+      <c r="Q32" s="114"/>
+      <c r="R32" s="114"/>
+      <c r="S32" s="114"/>
+      <c r="T32" s="114"/>
+      <c r="U32" s="114"/>
+      <c r="V32" s="114"/>
+      <c r="W32" s="114"/>
       <c r="X32" s="75"/>
       <c r="Y32" s="25"/>
     </row>
     <row r="33" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111" t="s">
+      <c r="A33" s="108" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="112"/>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="113"/>
-      <c r="F33" s="114"/>
-      <c r="G33" s="114"/>
-      <c r="H33" s="114"/>
-      <c r="I33" s="114"/>
-      <c r="J33" s="114"/>
-      <c r="K33" s="114"/>
-      <c r="L33" s="114"/>
-      <c r="M33" s="115"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="109"/>
+      <c r="E33" s="110"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="112"/>
+      <c r="I33" s="112"/>
+      <c r="J33" s="112"/>
+      <c r="K33" s="112"/>
+      <c r="L33" s="112"/>
+      <c r="M33" s="113"/>
       <c r="N33" s="22"/>
-      <c r="O33" s="163"/>
-      <c r="P33" s="163"/>
-      <c r="Q33" s="163"/>
-      <c r="R33" s="163"/>
-      <c r="S33" s="163"/>
-      <c r="T33" s="163"/>
-      <c r="U33" s="163"/>
-      <c r="V33" s="163"/>
-      <c r="W33" s="163"/>
+      <c r="O33" s="114"/>
+      <c r="P33" s="114"/>
+      <c r="Q33" s="114"/>
+      <c r="R33" s="114"/>
+      <c r="S33" s="114"/>
+      <c r="T33" s="114"/>
+      <c r="U33" s="114"/>
+      <c r="V33" s="114"/>
+      <c r="W33" s="114"/>
       <c r="X33" s="22"/>
       <c r="Y33" s="13"/>
     </row>
     <row r="34" spans="1:25" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="110"/>
-      <c r="B34" s="110"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="115"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -8485,46 +8486,46 @@
       <c r="L34" s="7"/>
       <c r="M34" s="7"/>
       <c r="N34" s="7"/>
-      <c r="O34" s="163"/>
-      <c r="P34" s="163"/>
-      <c r="Q34" s="163"/>
-      <c r="R34" s="163"/>
-      <c r="S34" s="163"/>
-      <c r="T34" s="163"/>
-      <c r="U34" s="163"/>
-      <c r="V34" s="163"/>
-      <c r="W34" s="163"/>
+      <c r="O34" s="114"/>
+      <c r="P34" s="114"/>
+      <c r="Q34" s="114"/>
+      <c r="R34" s="114"/>
+      <c r="S34" s="114"/>
+      <c r="T34" s="114"/>
+      <c r="U34" s="114"/>
+      <c r="V34" s="114"/>
+      <c r="W34" s="114"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="7"/>
     </row>
     <row r="35" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="108" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="112"/>
-      <c r="C35" s="112"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="114" t="s">
+      <c r="B35" s="109"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="114"/>
-      <c r="H35" s="114"/>
-      <c r="I35" s="114"/>
-      <c r="J35" s="114"/>
-      <c r="K35" s="114"/>
-      <c r="L35" s="114"/>
-      <c r="M35" s="115"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="112"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="112"/>
+      <c r="M35" s="113"/>
       <c r="N35" s="22"/>
-      <c r="O35" s="163"/>
-      <c r="P35" s="163"/>
-      <c r="Q35" s="163"/>
-      <c r="R35" s="163"/>
-      <c r="S35" s="163"/>
-      <c r="T35" s="163"/>
-      <c r="U35" s="163"/>
-      <c r="V35" s="163"/>
-      <c r="W35" s="163"/>
+      <c r="O35" s="114"/>
+      <c r="P35" s="114"/>
+      <c r="Q35" s="114"/>
+      <c r="R35" s="114"/>
+      <c r="S35" s="114"/>
+      <c r="T35" s="114"/>
+      <c r="U35" s="114"/>
+      <c r="V35" s="114"/>
+      <c r="W35" s="114"/>
       <c r="X35" s="75"/>
       <c r="Y35" s="12"/>
     </row>
@@ -8543,36 +8544,36 @@
       <c r="L36" s="23"/>
       <c r="M36" s="23"/>
       <c r="N36" s="23"/>
-      <c r="O36" s="163"/>
-      <c r="P36" s="163"/>
-      <c r="Q36" s="163"/>
-      <c r="R36" s="163"/>
-      <c r="S36" s="163"/>
-      <c r="T36" s="163"/>
-      <c r="U36" s="163"/>
-      <c r="V36" s="163"/>
-      <c r="W36" s="163"/>
+      <c r="O36" s="114"/>
+      <c r="P36" s="114"/>
+      <c r="Q36" s="114"/>
+      <c r="R36" s="114"/>
+      <c r="S36" s="114"/>
+      <c r="T36" s="114"/>
+      <c r="U36" s="114"/>
+      <c r="V36" s="114"/>
+      <c r="W36" s="114"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="5"/>
     </row>
     <row r="37" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="111" t="s">
+      <c r="A37" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="112"/>
-      <c r="C37" s="112"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="114" t="s">
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="109"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="114"/>
-      <c r="H37" s="114"/>
-      <c r="I37" s="114"/>
-      <c r="J37" s="114"/>
-      <c r="K37" s="114"/>
-      <c r="L37" s="114"/>
-      <c r="M37" s="115"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="112"/>
+      <c r="M37" s="113"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
       <c r="P37" s="100"/>
@@ -8614,21 +8615,21 @@
       <c r="Y38" s="5"/>
     </row>
     <row r="39" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="111" t="s">
+      <c r="A39" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="112"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="113"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="114"/>
-      <c r="H39" s="114"/>
-      <c r="I39" s="114"/>
-      <c r="J39" s="114"/>
-      <c r="K39" s="114"/>
-      <c r="L39" s="114"/>
-      <c r="M39" s="115"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="109"/>
+      <c r="E39" s="110"/>
+      <c r="F39" s="111"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="112"/>
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="112"/>
+      <c r="M39" s="113"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
       <c r="P39" s="90"/>
@@ -8643,8 +8644,8 @@
       <c r="Y39" s="13"/>
     </row>
     <row r="40" spans="1:25" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="110"/>
-      <c r="B40" s="110"/>
+      <c r="A40" s="115"/>
+      <c r="B40" s="115"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -8670,21 +8671,21 @@
       <c r="Y40" s="6"/>
     </row>
     <row r="41" spans="1:25" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="108" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="118"/>
-      <c r="G41" s="114"/>
-      <c r="H41" s="114"/>
-      <c r="I41" s="114"/>
-      <c r="J41" s="114"/>
-      <c r="K41" s="114"/>
-      <c r="L41" s="114"/>
-      <c r="M41" s="115"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="112"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="112"/>
+      <c r="M41" s="113"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
       <c r="P41" s="90"/>
@@ -8726,21 +8727,21 @@
       <c r="Y42" s="79"/>
     </row>
     <row r="43" spans="1:25" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="111" t="s">
+      <c r="A43" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="113"/>
-      <c r="F43" s="118"/>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114"/>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114"/>
-      <c r="M43" s="115"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="109"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="111"/>
+      <c r="G43" s="112"/>
+      <c r="H43" s="112"/>
+      <c r="I43" s="112"/>
+      <c r="J43" s="112"/>
+      <c r="K43" s="112"/>
+      <c r="L43" s="112"/>
+      <c r="M43" s="113"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
       <c r="P43" s="90"/>
@@ -8782,23 +8783,23 @@
       <c r="Y44" s="25"/>
     </row>
     <row r="45" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="111" t="s">
+      <c r="A45" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="112"/>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="114" t="s">
+      <c r="B45" s="109"/>
+      <c r="C45" s="109"/>
+      <c r="D45" s="109"/>
+      <c r="E45" s="110"/>
+      <c r="F45" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="114"/>
-      <c r="H45" s="114"/>
-      <c r="I45" s="114"/>
-      <c r="J45" s="114"/>
-      <c r="K45" s="114"/>
-      <c r="L45" s="114"/>
-      <c r="M45" s="115"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="112"/>
+      <c r="M45" s="113"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
       <c r="P45" s="90"/>
@@ -8840,21 +8841,21 @@
       <c r="Y46" s="25"/>
     </row>
     <row r="47" spans="1:25" s="1" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="111" t="s">
+      <c r="A47" s="108" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="112"/>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="113"/>
-      <c r="F47" s="114"/>
-      <c r="G47" s="114"/>
-      <c r="H47" s="114"/>
-      <c r="I47" s="114"/>
-      <c r="J47" s="114"/>
-      <c r="K47" s="114"/>
-      <c r="L47" s="114"/>
-      <c r="M47" s="115"/>
+      <c r="B47" s="109"/>
+      <c r="C47" s="109"/>
+      <c r="D47" s="109"/>
+      <c r="E47" s="110"/>
+      <c r="F47" s="112"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
+      <c r="J47" s="112"/>
+      <c r="K47" s="112"/>
+      <c r="L47" s="112"/>
+      <c r="M47" s="113"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
       <c r="P47" s="90"/>
@@ -8869,8 +8870,8 @@
       <c r="Y47" s="13"/>
     </row>
     <row r="48" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="143"/>
-      <c r="B48" s="143"/>
+      <c r="A48" s="124"/>
+      <c r="B48" s="124"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -8976,8 +8977,8 @@
       <c r="Y51" s="85"/>
     </row>
     <row r="52" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="156"/>
-      <c r="B52" s="156"/>
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
@@ -9003,8 +9004,8 @@
       <c r="Y52" s="5"/>
     </row>
     <row r="53" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="156"/>
-      <c r="B53" s="156"/>
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -9030,8 +9031,8 @@
       <c r="Y53" s="6"/>
     </row>
     <row r="54" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="110"/>
-      <c r="B54" s="110"/>
+      <c r="A54" s="115"/>
+      <c r="B54" s="115"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -9057,8 +9058,8 @@
       <c r="Y54" s="6"/>
     </row>
     <row r="55" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="110"/>
-      <c r="B55" s="110"/>
+      <c r="A55" s="115"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -9084,8 +9085,8 @@
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="110"/>
-      <c r="B56" s="110"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="115"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -9111,8 +9112,8 @@
       <c r="Y56" s="6"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A57" s="110"/>
-      <c r="B57" s="110"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="115"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -9192,35 +9193,35 @@
       <c r="Y59" s="4"/>
     </row>
     <row r="60" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="158"/>
-      <c r="B60" s="158"/>
-      <c r="C60" s="157"/>
-      <c r="D60" s="157"/>
-      <c r="E60" s="157"/>
-      <c r="F60" s="157"/>
-      <c r="G60" s="157"/>
-      <c r="H60" s="157"/>
-      <c r="I60" s="157"/>
-      <c r="J60" s="157"/>
-      <c r="K60" s="157"/>
-      <c r="L60" s="157"/>
-      <c r="M60" s="157"/>
-      <c r="N60" s="157"/>
-      <c r="O60" s="157"/>
-      <c r="P60" s="157"/>
-      <c r="Q60" s="157"/>
-      <c r="R60" s="157"/>
-      <c r="S60" s="157"/>
-      <c r="T60" s="157"/>
-      <c r="U60" s="157"/>
-      <c r="V60" s="157"/>
-      <c r="W60" s="157"/>
-      <c r="X60" s="157"/>
-      <c r="Y60" s="157"/>
+      <c r="A60" s="122"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="120"/>
+      <c r="D60" s="120"/>
+      <c r="E60" s="120"/>
+      <c r="F60" s="120"/>
+      <c r="G60" s="120"/>
+      <c r="H60" s="120"/>
+      <c r="I60" s="120"/>
+      <c r="J60" s="120"/>
+      <c r="K60" s="120"/>
+      <c r="L60" s="120"/>
+      <c r="M60" s="120"/>
+      <c r="N60" s="120"/>
+      <c r="O60" s="120"/>
+      <c r="P60" s="120"/>
+      <c r="Q60" s="120"/>
+      <c r="R60" s="120"/>
+      <c r="S60" s="120"/>
+      <c r="T60" s="120"/>
+      <c r="U60" s="120"/>
+      <c r="V60" s="120"/>
+      <c r="W60" s="120"/>
+      <c r="X60" s="120"/>
+      <c r="Y60" s="120"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A61" s="156"/>
-      <c r="B61" s="156"/>
+      <c r="A61" s="121"/>
+      <c r="B61" s="121"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
@@ -9246,8 +9247,8 @@
       <c r="Y61" s="5"/>
     </row>
     <row r="62" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="156"/>
-      <c r="B62" s="156"/>
+      <c r="A62" s="121"/>
+      <c r="B62" s="121"/>
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -9273,8 +9274,8 @@
       <c r="Y62" s="6"/>
     </row>
     <row r="63" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="110"/>
-      <c r="B63" s="110"/>
+      <c r="A63" s="115"/>
+      <c r="B63" s="115"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
       <c r="E63" s="6"/>
@@ -9300,8 +9301,8 @@
       <c r="Y63" s="6"/>
     </row>
     <row r="64" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="110"/>
-      <c r="B64" s="110"/>
+      <c r="A64" s="115"/>
+      <c r="B64" s="115"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
@@ -9327,8 +9328,8 @@
       <c r="Y64" s="7"/>
     </row>
     <row r="65" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="110"/>
-      <c r="B65" s="110"/>
+      <c r="A65" s="115"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
       <c r="E65" s="6"/>
@@ -9354,8 +9355,8 @@
       <c r="Y65" s="6"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A66" s="110"/>
-      <c r="B66" s="110"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="115"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -9489,35 +9490,35 @@
       <c r="Y70" s="4"/>
     </row>
     <row r="71" spans="1:25" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="159"/>
-      <c r="B71" s="159"/>
-      <c r="C71" s="157"/>
-      <c r="D71" s="157"/>
-      <c r="E71" s="157"/>
-      <c r="F71" s="157"/>
-      <c r="G71" s="157"/>
-      <c r="H71" s="157"/>
-      <c r="I71" s="157"/>
-      <c r="J71" s="157"/>
-      <c r="K71" s="157"/>
-      <c r="L71" s="157"/>
-      <c r="M71" s="157"/>
-      <c r="N71" s="157"/>
-      <c r="O71" s="157"/>
-      <c r="P71" s="157"/>
-      <c r="Q71" s="157"/>
-      <c r="R71" s="157"/>
-      <c r="S71" s="157"/>
-      <c r="T71" s="157"/>
-      <c r="U71" s="157"/>
-      <c r="V71" s="157"/>
-      <c r="W71" s="157"/>
-      <c r="X71" s="157"/>
-      <c r="Y71" s="157"/>
+      <c r="A71" s="123"/>
+      <c r="B71" s="123"/>
+      <c r="C71" s="120"/>
+      <c r="D71" s="120"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="120"/>
+      <c r="G71" s="120"/>
+      <c r="H71" s="120"/>
+      <c r="I71" s="120"/>
+      <c r="J71" s="120"/>
+      <c r="K71" s="120"/>
+      <c r="L71" s="120"/>
+      <c r="M71" s="120"/>
+      <c r="N71" s="120"/>
+      <c r="O71" s="120"/>
+      <c r="P71" s="120"/>
+      <c r="Q71" s="120"/>
+      <c r="R71" s="120"/>
+      <c r="S71" s="120"/>
+      <c r="T71" s="120"/>
+      <c r="U71" s="120"/>
+      <c r="V71" s="120"/>
+      <c r="W71" s="120"/>
+      <c r="X71" s="120"/>
+      <c r="Y71" s="120"/>
     </row>
     <row r="72" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="156"/>
-      <c r="B72" s="156"/>
+      <c r="A72" s="121"/>
+      <c r="B72" s="121"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
@@ -9543,8 +9544,8 @@
       <c r="Y72" s="5"/>
     </row>
     <row r="73" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="156"/>
-      <c r="B73" s="156"/>
+      <c r="A73" s="121"/>
+      <c r="B73" s="121"/>
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -9570,8 +9571,8 @@
       <c r="Y73" s="9"/>
     </row>
     <row r="74" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="110"/>
-      <c r="B74" s="110"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="115"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -9597,8 +9598,8 @@
       <c r="Y74" s="9"/>
     </row>
     <row r="75" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="110"/>
-      <c r="B75" s="110"/>
+      <c r="A75" s="115"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -9624,8 +9625,8 @@
       <c r="Y75" s="10"/>
     </row>
     <row r="76" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="110"/>
-      <c r="B76" s="110"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="115"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
@@ -9651,8 +9652,8 @@
       <c r="Y76" s="9"/>
     </row>
     <row r="77" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="110"/>
-      <c r="B77" s="110"/>
+      <c r="A77" s="115"/>
+      <c r="B77" s="115"/>
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -9732,35 +9733,35 @@
       <c r="Y79" s="4"/>
     </row>
     <row r="80" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="158"/>
-      <c r="B80" s="158"/>
-      <c r="C80" s="157"/>
-      <c r="D80" s="157"/>
-      <c r="E80" s="157"/>
-      <c r="F80" s="157"/>
-      <c r="G80" s="157"/>
-      <c r="H80" s="157"/>
-      <c r="I80" s="157"/>
-      <c r="J80" s="157"/>
-      <c r="K80" s="157"/>
-      <c r="L80" s="157"/>
-      <c r="M80" s="157"/>
-      <c r="N80" s="157"/>
-      <c r="O80" s="157"/>
-      <c r="P80" s="157"/>
-      <c r="Q80" s="157"/>
-      <c r="R80" s="157"/>
-      <c r="S80" s="157"/>
-      <c r="T80" s="157"/>
-      <c r="U80" s="157"/>
-      <c r="V80" s="157"/>
-      <c r="W80" s="157"/>
-      <c r="X80" s="157"/>
-      <c r="Y80" s="157"/>
+      <c r="A80" s="122"/>
+      <c r="B80" s="122"/>
+      <c r="C80" s="120"/>
+      <c r="D80" s="120"/>
+      <c r="E80" s="120"/>
+      <c r="F80" s="120"/>
+      <c r="G80" s="120"/>
+      <c r="H80" s="120"/>
+      <c r="I80" s="120"/>
+      <c r="J80" s="120"/>
+      <c r="K80" s="120"/>
+      <c r="L80" s="120"/>
+      <c r="M80" s="120"/>
+      <c r="N80" s="120"/>
+      <c r="O80" s="120"/>
+      <c r="P80" s="120"/>
+      <c r="Q80" s="120"/>
+      <c r="R80" s="120"/>
+      <c r="S80" s="120"/>
+      <c r="T80" s="120"/>
+      <c r="U80" s="120"/>
+      <c r="V80" s="120"/>
+      <c r="W80" s="120"/>
+      <c r="X80" s="120"/>
+      <c r="Y80" s="120"/>
     </row>
     <row r="81" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="156"/>
-      <c r="B81" s="156"/>
+      <c r="A81" s="121"/>
+      <c r="B81" s="121"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -9786,8 +9787,8 @@
       <c r="Y81" s="5"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A82" s="156"/>
-      <c r="B82" s="156"/>
+      <c r="A82" s="121"/>
+      <c r="B82" s="121"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
@@ -9813,8 +9814,8 @@
       <c r="Y82" s="6"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A83" s="110"/>
-      <c r="B83" s="110"/>
+      <c r="A83" s="115"/>
+      <c r="B83" s="115"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
@@ -9840,8 +9841,8 @@
       <c r="Y83" s="6"/>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A84" s="110"/>
-      <c r="B84" s="110"/>
+      <c r="A84" s="115"/>
+      <c r="B84" s="115"/>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -9867,8 +9868,8 @@
       <c r="Y84" s="7"/>
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A85" s="110"/>
-      <c r="B85" s="110"/>
+      <c r="A85" s="115"/>
+      <c r="B85" s="115"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
@@ -9894,8 +9895,8 @@
       <c r="Y85" s="6"/>
     </row>
     <row r="86" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A86" s="110"/>
-      <c r="B86" s="110"/>
+      <c r="A86" s="115"/>
+      <c r="B86" s="115"/>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -9975,35 +9976,35 @@
       <c r="Y88" s="4"/>
     </row>
     <row r="89" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="158"/>
-      <c r="B89" s="158"/>
-      <c r="C89" s="157"/>
-      <c r="D89" s="157"/>
-      <c r="E89" s="157"/>
-      <c r="F89" s="157"/>
-      <c r="G89" s="157"/>
-      <c r="H89" s="157"/>
-      <c r="I89" s="157"/>
-      <c r="J89" s="157"/>
-      <c r="K89" s="157"/>
-      <c r="L89" s="157"/>
-      <c r="M89" s="157"/>
-      <c r="N89" s="157"/>
-      <c r="O89" s="157"/>
-      <c r="P89" s="157"/>
-      <c r="Q89" s="157"/>
-      <c r="R89" s="157"/>
-      <c r="S89" s="157"/>
-      <c r="T89" s="157"/>
-      <c r="U89" s="157"/>
-      <c r="V89" s="157"/>
-      <c r="W89" s="157"/>
-      <c r="X89" s="157"/>
-      <c r="Y89" s="157"/>
+      <c r="A89" s="122"/>
+      <c r="B89" s="122"/>
+      <c r="C89" s="120"/>
+      <c r="D89" s="120"/>
+      <c r="E89" s="120"/>
+      <c r="F89" s="120"/>
+      <c r="G89" s="120"/>
+      <c r="H89" s="120"/>
+      <c r="I89" s="120"/>
+      <c r="J89" s="120"/>
+      <c r="K89" s="120"/>
+      <c r="L89" s="120"/>
+      <c r="M89" s="120"/>
+      <c r="N89" s="120"/>
+      <c r="O89" s="120"/>
+      <c r="P89" s="120"/>
+      <c r="Q89" s="120"/>
+      <c r="R89" s="120"/>
+      <c r="S89" s="120"/>
+      <c r="T89" s="120"/>
+      <c r="U89" s="120"/>
+      <c r="V89" s="120"/>
+      <c r="W89" s="120"/>
+      <c r="X89" s="120"/>
+      <c r="Y89" s="120"/>
     </row>
     <row r="90" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="156"/>
-      <c r="B90" s="156"/>
+      <c r="A90" s="121"/>
+      <c r="B90" s="121"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -10029,8 +10030,8 @@
       <c r="Y90" s="5"/>
     </row>
     <row r="91" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="156"/>
-      <c r="B91" s="156"/>
+      <c r="A91" s="121"/>
+      <c r="B91" s="121"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -10056,8 +10057,8 @@
       <c r="Y91" s="9"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A92" s="110"/>
-      <c r="B92" s="110"/>
+      <c r="A92" s="115"/>
+      <c r="B92" s="115"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="6"/>
@@ -10083,8 +10084,8 @@
       <c r="Y92" s="6"/>
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A93" s="110"/>
-      <c r="B93" s="110"/>
+      <c r="A93" s="115"/>
+      <c r="B93" s="115"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -10110,8 +10111,8 @@
       <c r="Y93" s="7"/>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A94" s="110"/>
-      <c r="B94" s="110"/>
+      <c r="A94" s="115"/>
+      <c r="B94" s="115"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="6"/>
@@ -10137,8 +10138,8 @@
       <c r="Y94" s="6"/>
     </row>
     <row r="95" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A95" s="110"/>
-      <c r="B95" s="110"/>
+      <c r="A95" s="115"/>
+      <c r="B95" s="115"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -10245,35 +10246,35 @@
       <c r="Y98" s="7"/>
     </row>
     <row r="99" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="158"/>
-      <c r="B99" s="158"/>
-      <c r="C99" s="157"/>
-      <c r="D99" s="157"/>
-      <c r="E99" s="157"/>
-      <c r="F99" s="157"/>
-      <c r="G99" s="157"/>
-      <c r="H99" s="157"/>
-      <c r="I99" s="157"/>
-      <c r="J99" s="157"/>
-      <c r="K99" s="157"/>
-      <c r="L99" s="157"/>
-      <c r="M99" s="157"/>
-      <c r="N99" s="157"/>
-      <c r="O99" s="157"/>
-      <c r="P99" s="157"/>
-      <c r="Q99" s="157"/>
-      <c r="R99" s="157"/>
-      <c r="S99" s="157"/>
-      <c r="T99" s="157"/>
-      <c r="U99" s="157"/>
-      <c r="V99" s="157"/>
-      <c r="W99" s="157"/>
-      <c r="X99" s="157"/>
-      <c r="Y99" s="157"/>
+      <c r="A99" s="122"/>
+      <c r="B99" s="122"/>
+      <c r="C99" s="120"/>
+      <c r="D99" s="120"/>
+      <c r="E99" s="120"/>
+      <c r="F99" s="120"/>
+      <c r="G99" s="120"/>
+      <c r="H99" s="120"/>
+      <c r="I99" s="120"/>
+      <c r="J99" s="120"/>
+      <c r="K99" s="120"/>
+      <c r="L99" s="120"/>
+      <c r="M99" s="120"/>
+      <c r="N99" s="120"/>
+      <c r="O99" s="120"/>
+      <c r="P99" s="120"/>
+      <c r="Q99" s="120"/>
+      <c r="R99" s="120"/>
+      <c r="S99" s="120"/>
+      <c r="T99" s="120"/>
+      <c r="U99" s="120"/>
+      <c r="V99" s="120"/>
+      <c r="W99" s="120"/>
+      <c r="X99" s="120"/>
+      <c r="Y99" s="120"/>
     </row>
     <row r="100" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="156"/>
-      <c r="B100" s="156"/>
+      <c r="A100" s="121"/>
+      <c r="B100" s="121"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
       <c r="E100" s="5"/>
@@ -10299,8 +10300,8 @@
       <c r="Y100" s="5"/>
     </row>
     <row r="101" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="156"/>
-      <c r="B101" s="156"/>
+      <c r="A101" s="121"/>
+      <c r="B101" s="121"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
@@ -10326,8 +10327,8 @@
       <c r="Y101" s="9"/>
     </row>
     <row r="102" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A102" s="110"/>
-      <c r="B102" s="110"/>
+      <c r="A102" s="115"/>
+      <c r="B102" s="115"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
@@ -10353,8 +10354,8 @@
       <c r="Y102" s="6"/>
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A103" s="110"/>
-      <c r="B103" s="110"/>
+      <c r="A103" s="115"/>
+      <c r="B103" s="115"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
@@ -10380,8 +10381,8 @@
       <c r="Y103" s="6"/>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A104" s="110"/>
-      <c r="B104" s="110"/>
+      <c r="A104" s="115"/>
+      <c r="B104" s="115"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
@@ -10407,8 +10408,8 @@
       <c r="Y104" s="6"/>
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A105" s="110"/>
-      <c r="B105" s="110"/>
+      <c r="A105" s="115"/>
+      <c r="B105" s="115"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
@@ -10488,35 +10489,35 @@
       <c r="Y107" s="6"/>
     </row>
     <row r="108" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="158"/>
-      <c r="B108" s="158"/>
-      <c r="C108" s="157"/>
-      <c r="D108" s="157"/>
-      <c r="E108" s="157"/>
-      <c r="F108" s="157"/>
-      <c r="G108" s="157"/>
-      <c r="H108" s="157"/>
-      <c r="I108" s="157"/>
-      <c r="J108" s="157"/>
-      <c r="K108" s="157"/>
-      <c r="L108" s="157"/>
-      <c r="M108" s="157"/>
-      <c r="N108" s="157"/>
-      <c r="O108" s="157"/>
-      <c r="P108" s="157"/>
-      <c r="Q108" s="157"/>
-      <c r="R108" s="157"/>
-      <c r="S108" s="157"/>
-      <c r="T108" s="157"/>
-      <c r="U108" s="157"/>
-      <c r="V108" s="157"/>
-      <c r="W108" s="157"/>
-      <c r="X108" s="157"/>
-      <c r="Y108" s="157"/>
+      <c r="A108" s="122"/>
+      <c r="B108" s="122"/>
+      <c r="C108" s="120"/>
+      <c r="D108" s="120"/>
+      <c r="E108" s="120"/>
+      <c r="F108" s="120"/>
+      <c r="G108" s="120"/>
+      <c r="H108" s="120"/>
+      <c r="I108" s="120"/>
+      <c r="J108" s="120"/>
+      <c r="K108" s="120"/>
+      <c r="L108" s="120"/>
+      <c r="M108" s="120"/>
+      <c r="N108" s="120"/>
+      <c r="O108" s="120"/>
+      <c r="P108" s="120"/>
+      <c r="Q108" s="120"/>
+      <c r="R108" s="120"/>
+      <c r="S108" s="120"/>
+      <c r="T108" s="120"/>
+      <c r="U108" s="120"/>
+      <c r="V108" s="120"/>
+      <c r="W108" s="120"/>
+      <c r="X108" s="120"/>
+      <c r="Y108" s="120"/>
     </row>
     <row r="109" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="156"/>
-      <c r="B109" s="156"/>
+      <c r="A109" s="121"/>
+      <c r="B109" s="121"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
       <c r="E109" s="5"/>
@@ -10542,8 +10543,8 @@
       <c r="Y109" s="5"/>
     </row>
     <row r="110" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="156"/>
-      <c r="B110" s="156"/>
+      <c r="A110" s="121"/>
+      <c r="B110" s="121"/>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
@@ -10569,8 +10570,8 @@
       <c r="Y110" s="9"/>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A111" s="110"/>
-      <c r="B111" s="110"/>
+      <c r="A111" s="115"/>
+      <c r="B111" s="115"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
@@ -10596,8 +10597,8 @@
       <c r="Y111" s="6"/>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A112" s="110"/>
-      <c r="B112" s="110"/>
+      <c r="A112" s="115"/>
+      <c r="B112" s="115"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
@@ -10623,8 +10624,8 @@
       <c r="Y112" s="6"/>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A113" s="110"/>
-      <c r="B113" s="110"/>
+      <c r="A113" s="115"/>
+      <c r="B113" s="115"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
@@ -10650,8 +10651,8 @@
       <c r="Y113" s="6"/>
     </row>
     <row r="114" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A114" s="110"/>
-      <c r="B114" s="110"/>
+      <c r="A114" s="115"/>
+      <c r="B114" s="115"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
@@ -10731,35 +10732,35 @@
       <c r="Y116" s="6"/>
     </row>
     <row r="117" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="158"/>
-      <c r="B117" s="158"/>
-      <c r="C117" s="157"/>
-      <c r="D117" s="157"/>
-      <c r="E117" s="157"/>
-      <c r="F117" s="157"/>
-      <c r="G117" s="157"/>
-      <c r="H117" s="157"/>
-      <c r="I117" s="157"/>
-      <c r="J117" s="157"/>
-      <c r="K117" s="157"/>
-      <c r="L117" s="157"/>
-      <c r="M117" s="157"/>
-      <c r="N117" s="157"/>
-      <c r="O117" s="157"/>
-      <c r="P117" s="157"/>
-      <c r="Q117" s="157"/>
-      <c r="R117" s="157"/>
-      <c r="S117" s="157"/>
-      <c r="T117" s="157"/>
-      <c r="U117" s="157"/>
-      <c r="V117" s="157"/>
-      <c r="W117" s="157"/>
-      <c r="X117" s="157"/>
-      <c r="Y117" s="157"/>
+      <c r="A117" s="122"/>
+      <c r="B117" s="122"/>
+      <c r="C117" s="120"/>
+      <c r="D117" s="120"/>
+      <c r="E117" s="120"/>
+      <c r="F117" s="120"/>
+      <c r="G117" s="120"/>
+      <c r="H117" s="120"/>
+      <c r="I117" s="120"/>
+      <c r="J117" s="120"/>
+      <c r="K117" s="120"/>
+      <c r="L117" s="120"/>
+      <c r="M117" s="120"/>
+      <c r="N117" s="120"/>
+      <c r="O117" s="120"/>
+      <c r="P117" s="120"/>
+      <c r="Q117" s="120"/>
+      <c r="R117" s="120"/>
+      <c r="S117" s="120"/>
+      <c r="T117" s="120"/>
+      <c r="U117" s="120"/>
+      <c r="V117" s="120"/>
+      <c r="W117" s="120"/>
+      <c r="X117" s="120"/>
+      <c r="Y117" s="120"/>
     </row>
     <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="156"/>
-      <c r="B118" s="156"/>
+      <c r="A118" s="121"/>
+      <c r="B118" s="121"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
@@ -10785,8 +10786,8 @@
       <c r="Y118" s="5"/>
     </row>
     <row r="119" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="156"/>
-      <c r="B119" s="156"/>
+      <c r="A119" s="121"/>
+      <c r="B119" s="121"/>
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="E119" s="9"/>
@@ -10812,8 +10813,8 @@
       <c r="Y119" s="9"/>
     </row>
     <row r="120" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A120" s="110"/>
-      <c r="B120" s="110"/>
+      <c r="A120" s="115"/>
+      <c r="B120" s="115"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
@@ -10839,8 +10840,8 @@
       <c r="Y120" s="6"/>
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A121" s="110"/>
-      <c r="B121" s="110"/>
+      <c r="A121" s="115"/>
+      <c r="B121" s="115"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
@@ -10866,8 +10867,8 @@
       <c r="Y121" s="6"/>
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A122" s="110"/>
-      <c r="B122" s="110"/>
+      <c r="A122" s="115"/>
+      <c r="B122" s="115"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
       <c r="E122" s="6"/>
@@ -10893,8 +10894,8 @@
       <c r="Y122" s="6"/>
     </row>
     <row r="123" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A123" s="110"/>
-      <c r="B123" s="110"/>
+      <c r="A123" s="115"/>
+      <c r="B123" s="115"/>
       <c r="C123" s="6"/>
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
@@ -11001,35 +11002,35 @@
       <c r="Y126" s="6"/>
     </row>
     <row r="127" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="158"/>
-      <c r="B127" s="158"/>
-      <c r="C127" s="157"/>
-      <c r="D127" s="157"/>
-      <c r="E127" s="157"/>
-      <c r="F127" s="157"/>
-      <c r="G127" s="157"/>
-      <c r="H127" s="157"/>
-      <c r="I127" s="157"/>
-      <c r="J127" s="157"/>
-      <c r="K127" s="157"/>
-      <c r="L127" s="157"/>
-      <c r="M127" s="157"/>
-      <c r="N127" s="157"/>
-      <c r="O127" s="157"/>
-      <c r="P127" s="157"/>
-      <c r="Q127" s="157"/>
-      <c r="R127" s="157"/>
-      <c r="S127" s="157"/>
-      <c r="T127" s="157"/>
-      <c r="U127" s="157"/>
-      <c r="V127" s="157"/>
-      <c r="W127" s="157"/>
-      <c r="X127" s="157"/>
-      <c r="Y127" s="157"/>
+      <c r="A127" s="122"/>
+      <c r="B127" s="122"/>
+      <c r="C127" s="120"/>
+      <c r="D127" s="120"/>
+      <c r="E127" s="120"/>
+      <c r="F127" s="120"/>
+      <c r="G127" s="120"/>
+      <c r="H127" s="120"/>
+      <c r="I127" s="120"/>
+      <c r="J127" s="120"/>
+      <c r="K127" s="120"/>
+      <c r="L127" s="120"/>
+      <c r="M127" s="120"/>
+      <c r="N127" s="120"/>
+      <c r="O127" s="120"/>
+      <c r="P127" s="120"/>
+      <c r="Q127" s="120"/>
+      <c r="R127" s="120"/>
+      <c r="S127" s="120"/>
+      <c r="T127" s="120"/>
+      <c r="U127" s="120"/>
+      <c r="V127" s="120"/>
+      <c r="W127" s="120"/>
+      <c r="X127" s="120"/>
+      <c r="Y127" s="120"/>
     </row>
     <row r="128" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="156"/>
-      <c r="B128" s="156"/>
+      <c r="A128" s="121"/>
+      <c r="B128" s="121"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
@@ -11055,8 +11056,8 @@
       <c r="Y128" s="5"/>
     </row>
     <row r="129" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="156"/>
-      <c r="B129" s="156"/>
+      <c r="A129" s="121"/>
+      <c r="B129" s="121"/>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -11082,8 +11083,8 @@
       <c r="Y129" s="9"/>
     </row>
     <row r="130" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A130" s="110"/>
-      <c r="B130" s="110"/>
+      <c r="A130" s="115"/>
+      <c r="B130" s="115"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
@@ -11109,8 +11110,8 @@
       <c r="Y130" s="6"/>
     </row>
     <row r="131" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A131" s="110"/>
-      <c r="B131" s="110"/>
+      <c r="A131" s="115"/>
+      <c r="B131" s="115"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
       <c r="E131" s="6"/>
@@ -11136,8 +11137,8 @@
       <c r="Y131" s="6"/>
     </row>
     <row r="132" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A132" s="110"/>
-      <c r="B132" s="110"/>
+      <c r="A132" s="115"/>
+      <c r="B132" s="115"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
@@ -11163,8 +11164,8 @@
       <c r="Y132" s="6"/>
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A133" s="110"/>
-      <c r="B133" s="110"/>
+      <c r="A133" s="115"/>
+      <c r="B133" s="115"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
@@ -11244,35 +11245,35 @@
       <c r="Y135" s="6"/>
     </row>
     <row r="136" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="158"/>
-      <c r="B136" s="158"/>
-      <c r="C136" s="157"/>
-      <c r="D136" s="157"/>
-      <c r="E136" s="157"/>
-      <c r="F136" s="157"/>
-      <c r="G136" s="157"/>
-      <c r="H136" s="157"/>
-      <c r="I136" s="157"/>
-      <c r="J136" s="157"/>
-      <c r="K136" s="157"/>
-      <c r="L136" s="157"/>
-      <c r="M136" s="157"/>
-      <c r="N136" s="157"/>
-      <c r="O136" s="157"/>
-      <c r="P136" s="157"/>
-      <c r="Q136" s="157"/>
-      <c r="R136" s="157"/>
-      <c r="S136" s="157"/>
-      <c r="T136" s="157"/>
-      <c r="U136" s="157"/>
-      <c r="V136" s="157"/>
-      <c r="W136" s="157"/>
-      <c r="X136" s="157"/>
-      <c r="Y136" s="157"/>
+      <c r="A136" s="122"/>
+      <c r="B136" s="122"/>
+      <c r="C136" s="120"/>
+      <c r="D136" s="120"/>
+      <c r="E136" s="120"/>
+      <c r="F136" s="120"/>
+      <c r="G136" s="120"/>
+      <c r="H136" s="120"/>
+      <c r="I136" s="120"/>
+      <c r="J136" s="120"/>
+      <c r="K136" s="120"/>
+      <c r="L136" s="120"/>
+      <c r="M136" s="120"/>
+      <c r="N136" s="120"/>
+      <c r="O136" s="120"/>
+      <c r="P136" s="120"/>
+      <c r="Q136" s="120"/>
+      <c r="R136" s="120"/>
+      <c r="S136" s="120"/>
+      <c r="T136" s="120"/>
+      <c r="U136" s="120"/>
+      <c r="V136" s="120"/>
+      <c r="W136" s="120"/>
+      <c r="X136" s="120"/>
+      <c r="Y136" s="120"/>
     </row>
     <row r="137" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="156"/>
-      <c r="B137" s="156"/>
+      <c r="A137" s="121"/>
+      <c r="B137" s="121"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
@@ -11298,8 +11299,8 @@
       <c r="Y137" s="5"/>
     </row>
     <row r="138" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="156"/>
-      <c r="B138" s="156"/>
+      <c r="A138" s="121"/>
+      <c r="B138" s="121"/>
       <c r="C138" s="9"/>
       <c r="D138" s="9"/>
       <c r="E138" s="9"/>
@@ -11325,8 +11326,8 @@
       <c r="Y138" s="9"/>
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A139" s="110"/>
-      <c r="B139" s="110"/>
+      <c r="A139" s="115"/>
+      <c r="B139" s="115"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
@@ -11352,8 +11353,8 @@
       <c r="Y139" s="6"/>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A140" s="110"/>
-      <c r="B140" s="110"/>
+      <c r="A140" s="115"/>
+      <c r="B140" s="115"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
       <c r="E140" s="6"/>
@@ -11379,8 +11380,8 @@
       <c r="Y140" s="6"/>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A141" s="110"/>
-      <c r="B141" s="110"/>
+      <c r="A141" s="115"/>
+      <c r="B141" s="115"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
       <c r="E141" s="6"/>
@@ -11406,8 +11407,8 @@
       <c r="Y141" s="6"/>
     </row>
     <row r="142" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A142" s="110"/>
-      <c r="B142" s="110"/>
+      <c r="A142" s="115"/>
+      <c r="B142" s="115"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
       <c r="E142" s="6"/>
@@ -11487,35 +11488,35 @@
       <c r="Y144" s="6"/>
     </row>
     <row r="145" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="158"/>
-      <c r="B145" s="158"/>
-      <c r="C145" s="157"/>
-      <c r="D145" s="157"/>
-      <c r="E145" s="157"/>
-      <c r="F145" s="157"/>
-      <c r="G145" s="157"/>
-      <c r="H145" s="157"/>
-      <c r="I145" s="157"/>
-      <c r="J145" s="157"/>
-      <c r="K145" s="157"/>
-      <c r="L145" s="157"/>
-      <c r="M145" s="157"/>
-      <c r="N145" s="157"/>
-      <c r="O145" s="157"/>
-      <c r="P145" s="157"/>
-      <c r="Q145" s="157"/>
-      <c r="R145" s="157"/>
-      <c r="S145" s="157"/>
-      <c r="T145" s="157"/>
-      <c r="U145" s="157"/>
-      <c r="V145" s="157"/>
-      <c r="W145" s="157"/>
-      <c r="X145" s="157"/>
-      <c r="Y145" s="157"/>
+      <c r="A145" s="122"/>
+      <c r="B145" s="122"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="120"/>
+      <c r="E145" s="120"/>
+      <c r="F145" s="120"/>
+      <c r="G145" s="120"/>
+      <c r="H145" s="120"/>
+      <c r="I145" s="120"/>
+      <c r="J145" s="120"/>
+      <c r="K145" s="120"/>
+      <c r="L145" s="120"/>
+      <c r="M145" s="120"/>
+      <c r="N145" s="120"/>
+      <c r="O145" s="120"/>
+      <c r="P145" s="120"/>
+      <c r="Q145" s="120"/>
+      <c r="R145" s="120"/>
+      <c r="S145" s="120"/>
+      <c r="T145" s="120"/>
+      <c r="U145" s="120"/>
+      <c r="V145" s="120"/>
+      <c r="W145" s="120"/>
+      <c r="X145" s="120"/>
+      <c r="Y145" s="120"/>
     </row>
     <row r="146" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="156"/>
-      <c r="B146" s="156"/>
+      <c r="A146" s="121"/>
+      <c r="B146" s="121"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
@@ -11541,8 +11542,8 @@
       <c r="Y146" s="5"/>
     </row>
     <row r="147" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="156"/>
-      <c r="B147" s="156"/>
+      <c r="A147" s="121"/>
+      <c r="B147" s="121"/>
       <c r="C147" s="9"/>
       <c r="D147" s="9"/>
       <c r="E147" s="9"/>
@@ -11568,8 +11569,8 @@
       <c r="Y147" s="9"/>
     </row>
     <row r="148" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A148" s="110"/>
-      <c r="B148" s="110"/>
+      <c r="A148" s="115"/>
+      <c r="B148" s="115"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
@@ -11595,8 +11596,8 @@
       <c r="Y148" s="6"/>
     </row>
     <row r="149" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A149" s="110"/>
-      <c r="B149" s="110"/>
+      <c r="A149" s="115"/>
+      <c r="B149" s="115"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
@@ -11622,8 +11623,8 @@
       <c r="Y149" s="6"/>
     </row>
     <row r="150" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A150" s="110"/>
-      <c r="B150" s="110"/>
+      <c r="A150" s="115"/>
+      <c r="B150" s="115"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
@@ -11649,8 +11650,8 @@
       <c r="Y150" s="6"/>
     </row>
     <row r="151" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A151" s="110"/>
-      <c r="B151" s="110"/>
+      <c r="A151" s="115"/>
+      <c r="B151" s="115"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
@@ -11730,35 +11731,35 @@
       <c r="Y153" s="4"/>
     </row>
     <row r="154" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="158"/>
-      <c r="B154" s="158"/>
-      <c r="C154" s="157"/>
-      <c r="D154" s="157"/>
-      <c r="E154" s="157"/>
-      <c r="F154" s="157"/>
-      <c r="G154" s="157"/>
-      <c r="H154" s="157"/>
-      <c r="I154" s="157"/>
-      <c r="J154" s="157"/>
-      <c r="K154" s="157"/>
-      <c r="L154" s="157"/>
-      <c r="M154" s="157"/>
-      <c r="N154" s="157"/>
-      <c r="O154" s="157"/>
-      <c r="P154" s="157"/>
-      <c r="Q154" s="157"/>
-      <c r="R154" s="157"/>
-      <c r="S154" s="157"/>
-      <c r="T154" s="157"/>
-      <c r="U154" s="157"/>
-      <c r="V154" s="157"/>
-      <c r="W154" s="157"/>
-      <c r="X154" s="157"/>
-      <c r="Y154" s="157"/>
+      <c r="A154" s="122"/>
+      <c r="B154" s="122"/>
+      <c r="C154" s="120"/>
+      <c r="D154" s="120"/>
+      <c r="E154" s="120"/>
+      <c r="F154" s="120"/>
+      <c r="G154" s="120"/>
+      <c r="H154" s="120"/>
+      <c r="I154" s="120"/>
+      <c r="J154" s="120"/>
+      <c r="K154" s="120"/>
+      <c r="L154" s="120"/>
+      <c r="M154" s="120"/>
+      <c r="N154" s="120"/>
+      <c r="O154" s="120"/>
+      <c r="P154" s="120"/>
+      <c r="Q154" s="120"/>
+      <c r="R154" s="120"/>
+      <c r="S154" s="120"/>
+      <c r="T154" s="120"/>
+      <c r="U154" s="120"/>
+      <c r="V154" s="120"/>
+      <c r="W154" s="120"/>
+      <c r="X154" s="120"/>
+      <c r="Y154" s="120"/>
     </row>
     <row r="155" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="156"/>
-      <c r="B155" s="156"/>
+      <c r="A155" s="121"/>
+      <c r="B155" s="121"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
       <c r="E155" s="5"/>
@@ -11784,8 +11785,8 @@
       <c r="Y155" s="5"/>
     </row>
     <row r="156" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="156"/>
-      <c r="B156" s="156"/>
+      <c r="A156" s="121"/>
+      <c r="B156" s="121"/>
       <c r="C156" s="9"/>
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
@@ -11811,8 +11812,8 @@
       <c r="Y156" s="9"/>
     </row>
     <row r="157" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A157" s="110"/>
-      <c r="B157" s="110"/>
+      <c r="A157" s="115"/>
+      <c r="B157" s="115"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="E157" s="6"/>
@@ -11838,8 +11839,8 @@
       <c r="Y157" s="6"/>
     </row>
     <row r="158" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A158" s="110"/>
-      <c r="B158" s="110"/>
+      <c r="A158" s="115"/>
+      <c r="B158" s="115"/>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
@@ -11865,8 +11866,8 @@
       <c r="Y158" s="6"/>
     </row>
     <row r="159" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A159" s="110"/>
-      <c r="B159" s="110"/>
+      <c r="A159" s="115"/>
+      <c r="B159" s="115"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="6"/>
@@ -11892,8 +11893,8 @@
       <c r="Y159" s="6"/>
     </row>
     <row r="160" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A160" s="110"/>
-      <c r="B160" s="110"/>
+      <c r="A160" s="115"/>
+      <c r="B160" s="115"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="E160" s="6"/>
@@ -11973,35 +11974,35 @@
       <c r="Y162" s="6"/>
     </row>
     <row r="163" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="158"/>
-      <c r="B163" s="158"/>
-      <c r="C163" s="157"/>
-      <c r="D163" s="157"/>
-      <c r="E163" s="157"/>
-      <c r="F163" s="157"/>
-      <c r="G163" s="157"/>
-      <c r="H163" s="157"/>
-      <c r="I163" s="157"/>
-      <c r="J163" s="157"/>
-      <c r="K163" s="157"/>
-      <c r="L163" s="157"/>
-      <c r="M163" s="157"/>
-      <c r="N163" s="157"/>
-      <c r="O163" s="157"/>
-      <c r="P163" s="157"/>
-      <c r="Q163" s="157"/>
-      <c r="R163" s="157"/>
-      <c r="S163" s="157"/>
-      <c r="T163" s="157"/>
-      <c r="U163" s="157"/>
-      <c r="V163" s="157"/>
-      <c r="W163" s="157"/>
-      <c r="X163" s="157"/>
-      <c r="Y163" s="157"/>
+      <c r="A163" s="122"/>
+      <c r="B163" s="122"/>
+      <c r="C163" s="120"/>
+      <c r="D163" s="120"/>
+      <c r="E163" s="120"/>
+      <c r="F163" s="120"/>
+      <c r="G163" s="120"/>
+      <c r="H163" s="120"/>
+      <c r="I163" s="120"/>
+      <c r="J163" s="120"/>
+      <c r="K163" s="120"/>
+      <c r="L163" s="120"/>
+      <c r="M163" s="120"/>
+      <c r="N163" s="120"/>
+      <c r="O163" s="120"/>
+      <c r="P163" s="120"/>
+      <c r="Q163" s="120"/>
+      <c r="R163" s="120"/>
+      <c r="S163" s="120"/>
+      <c r="T163" s="120"/>
+      <c r="U163" s="120"/>
+      <c r="V163" s="120"/>
+      <c r="W163" s="120"/>
+      <c r="X163" s="120"/>
+      <c r="Y163" s="120"/>
     </row>
     <row r="164" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="156"/>
-      <c r="B164" s="156"/>
+      <c r="A164" s="121"/>
+      <c r="B164" s="121"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
       <c r="E164" s="5"/>
@@ -12027,8 +12028,8 @@
       <c r="Y164" s="5"/>
     </row>
     <row r="165" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="156"/>
-      <c r="B165" s="156"/>
+      <c r="A165" s="121"/>
+      <c r="B165" s="121"/>
       <c r="C165" s="9"/>
       <c r="D165" s="9"/>
       <c r="E165" s="9"/>
@@ -12054,8 +12055,8 @@
       <c r="Y165" s="9"/>
     </row>
     <row r="166" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A166" s="110"/>
-      <c r="B166" s="110"/>
+      <c r="A166" s="115"/>
+      <c r="B166" s="115"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="E166" s="6"/>
@@ -12081,8 +12082,8 @@
       <c r="Y166" s="6"/>
     </row>
     <row r="167" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A167" s="110"/>
-      <c r="B167" s="110"/>
+      <c r="A167" s="115"/>
+      <c r="B167" s="115"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="E167" s="6"/>
@@ -12108,8 +12109,8 @@
       <c r="Y167" s="6"/>
     </row>
     <row r="168" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A168" s="110"/>
-      <c r="B168" s="110"/>
+      <c r="A168" s="115"/>
+      <c r="B168" s="115"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="E168" s="6"/>
@@ -12135,8 +12136,8 @@
       <c r="Y168" s="6"/>
     </row>
     <row r="169" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A169" s="110"/>
-      <c r="B169" s="110"/>
+      <c r="A169" s="115"/>
+      <c r="B169" s="115"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="E169" s="6"/>
@@ -12216,35 +12217,35 @@
       <c r="Y171" s="6"/>
     </row>
     <row r="172" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="158"/>
-      <c r="B172" s="158"/>
-      <c r="C172" s="157"/>
-      <c r="D172" s="157"/>
-      <c r="E172" s="157"/>
-      <c r="F172" s="157"/>
-      <c r="G172" s="157"/>
-      <c r="H172" s="157"/>
-      <c r="I172" s="157"/>
-      <c r="J172" s="157"/>
-      <c r="K172" s="157"/>
-      <c r="L172" s="157"/>
-      <c r="M172" s="157"/>
-      <c r="N172" s="157"/>
-      <c r="O172" s="157"/>
-      <c r="P172" s="157"/>
-      <c r="Q172" s="157"/>
-      <c r="R172" s="157"/>
-      <c r="S172" s="157"/>
-      <c r="T172" s="157"/>
-      <c r="U172" s="157"/>
-      <c r="V172" s="157"/>
-      <c r="W172" s="157"/>
-      <c r="X172" s="157"/>
-      <c r="Y172" s="157"/>
+      <c r="A172" s="122"/>
+      <c r="B172" s="122"/>
+      <c r="C172" s="120"/>
+      <c r="D172" s="120"/>
+      <c r="E172" s="120"/>
+      <c r="F172" s="120"/>
+      <c r="G172" s="120"/>
+      <c r="H172" s="120"/>
+      <c r="I172" s="120"/>
+      <c r="J172" s="120"/>
+      <c r="K172" s="120"/>
+      <c r="L172" s="120"/>
+      <c r="M172" s="120"/>
+      <c r="N172" s="120"/>
+      <c r="O172" s="120"/>
+      <c r="P172" s="120"/>
+      <c r="Q172" s="120"/>
+      <c r="R172" s="120"/>
+      <c r="S172" s="120"/>
+      <c r="T172" s="120"/>
+      <c r="U172" s="120"/>
+      <c r="V172" s="120"/>
+      <c r="W172" s="120"/>
+      <c r="X172" s="120"/>
+      <c r="Y172" s="120"/>
     </row>
     <row r="173" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="156"/>
-      <c r="B173" s="156"/>
+      <c r="A173" s="121"/>
+      <c r="B173" s="121"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
       <c r="E173" s="5"/>
@@ -12270,8 +12271,8 @@
       <c r="Y173" s="5"/>
     </row>
     <row r="174" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="156"/>
-      <c r="B174" s="156"/>
+      <c r="A174" s="121"/>
+      <c r="B174" s="121"/>
       <c r="C174" s="9"/>
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
@@ -12297,8 +12298,8 @@
       <c r="Y174" s="9"/>
     </row>
     <row r="175" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A175" s="110"/>
-      <c r="B175" s="110"/>
+      <c r="A175" s="115"/>
+      <c r="B175" s="115"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
@@ -12324,8 +12325,8 @@
       <c r="Y175" s="6"/>
     </row>
     <row r="176" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A176" s="110"/>
-      <c r="B176" s="110"/>
+      <c r="A176" s="115"/>
+      <c r="B176" s="115"/>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="E176" s="6"/>
@@ -12351,8 +12352,8 @@
       <c r="Y176" s="6"/>
     </row>
     <row r="177" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A177" s="110"/>
-      <c r="B177" s="110"/>
+      <c r="A177" s="115"/>
+      <c r="B177" s="115"/>
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="E177" s="6"/>
@@ -12378,8 +12379,8 @@
       <c r="Y177" s="6"/>
     </row>
     <row r="178" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A178" s="110"/>
-      <c r="B178" s="110"/>
+      <c r="A178" s="115"/>
+      <c r="B178" s="115"/>
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="E178" s="6"/>
@@ -12459,35 +12460,35 @@
       <c r="Y180" s="6"/>
     </row>
     <row r="181" spans="1:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="158"/>
-      <c r="B181" s="158"/>
-      <c r="C181" s="157"/>
-      <c r="D181" s="157"/>
-      <c r="E181" s="157"/>
-      <c r="F181" s="157"/>
-      <c r="G181" s="157"/>
-      <c r="H181" s="157"/>
-      <c r="I181" s="157"/>
-      <c r="J181" s="157"/>
-      <c r="K181" s="157"/>
-      <c r="L181" s="157"/>
-      <c r="M181" s="157"/>
-      <c r="N181" s="157"/>
-      <c r="O181" s="157"/>
-      <c r="P181" s="157"/>
-      <c r="Q181" s="157"/>
-      <c r="R181" s="157"/>
-      <c r="S181" s="157"/>
-      <c r="T181" s="157"/>
-      <c r="U181" s="157"/>
-      <c r="V181" s="157"/>
-      <c r="W181" s="157"/>
-      <c r="X181" s="157"/>
-      <c r="Y181" s="157"/>
+      <c r="A181" s="122"/>
+      <c r="B181" s="122"/>
+      <c r="C181" s="120"/>
+      <c r="D181" s="120"/>
+      <c r="E181" s="120"/>
+      <c r="F181" s="120"/>
+      <c r="G181" s="120"/>
+      <c r="H181" s="120"/>
+      <c r="I181" s="120"/>
+      <c r="J181" s="120"/>
+      <c r="K181" s="120"/>
+      <c r="L181" s="120"/>
+      <c r="M181" s="120"/>
+      <c r="N181" s="120"/>
+      <c r="O181" s="120"/>
+      <c r="P181" s="120"/>
+      <c r="Q181" s="120"/>
+      <c r="R181" s="120"/>
+      <c r="S181" s="120"/>
+      <c r="T181" s="120"/>
+      <c r="U181" s="120"/>
+      <c r="V181" s="120"/>
+      <c r="W181" s="120"/>
+      <c r="X181" s="120"/>
+      <c r="Y181" s="120"/>
     </row>
     <row r="182" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="156"/>
-      <c r="B182" s="156"/>
+      <c r="A182" s="121"/>
+      <c r="B182" s="121"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
       <c r="E182" s="5"/>
@@ -12513,8 +12514,8 @@
       <c r="Y182" s="5"/>
     </row>
     <row r="183" spans="1:25" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="156"/>
-      <c r="B183" s="156"/>
+      <c r="A183" s="121"/>
+      <c r="B183" s="121"/>
       <c r="C183" s="9"/>
       <c r="D183" s="9"/>
       <c r="E183" s="9"/>
@@ -12540,8 +12541,8 @@
       <c r="Y183" s="9"/>
     </row>
     <row r="184" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A184" s="110"/>
-      <c r="B184" s="110"/>
+      <c r="A184" s="115"/>
+      <c r="B184" s="115"/>
       <c r="C184" s="6"/>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
@@ -12567,8 +12568,8 @@
       <c r="Y184" s="6"/>
     </row>
     <row r="185" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A185" s="110"/>
-      <c r="B185" s="110"/>
+      <c r="A185" s="115"/>
+      <c r="B185" s="115"/>
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
@@ -12594,8 +12595,8 @@
       <c r="Y185" s="6"/>
     </row>
     <row r="186" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A186" s="110"/>
-      <c r="B186" s="110"/>
+      <c r="A186" s="115"/>
+      <c r="B186" s="115"/>
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="E186" s="6"/>
@@ -12621,8 +12622,8 @@
       <c r="Y186" s="6"/>
     </row>
     <row r="187" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A187" s="110"/>
-      <c r="B187" s="110"/>
+      <c r="A187" s="115"/>
+      <c r="B187" s="115"/>
       <c r="C187" s="6"/>
       <c r="D187" s="6"/>
       <c r="E187" s="6"/>
@@ -43834,6 +43835,158 @@
     </row>
   </sheetData>
   <mergeCells count="176">
+    <mergeCell ref="A3:W3"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="F37:M37"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="F47:M47"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O6:R6"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="O10:S10"/>
+    <mergeCell ref="O11:S11"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="Q13:W13"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C71:Y71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C60:Y60"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C80:Y80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="A157:B157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A175:B175"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A163:B163"/>
+    <mergeCell ref="A164:B164"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="A181:B181"/>
+    <mergeCell ref="C181:Y181"/>
+    <mergeCell ref="C172:Y172"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="C154:Y154"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="C145:Y145"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="C136:Y136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="C127:Y127"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C163:Y163"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="C108:Y108"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="C99:Y99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="C89:Y89"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="C117:Y117"/>
+    <mergeCell ref="A118:B118"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:R1"/>
@@ -43858,158 +44011,6 @@
     <mergeCell ref="A25:S26"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="A4:W4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C163:Y163"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="C108:Y108"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="C99:Y99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="C89:Y89"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="C117:Y117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="C154:Y154"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="C145:Y145"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="C136:Y136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="C127:Y127"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A181:B181"/>
-    <mergeCell ref="C181:Y181"/>
-    <mergeCell ref="C172:Y172"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="A157:B157"/>
-    <mergeCell ref="A158:B158"/>
-    <mergeCell ref="A159:B159"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="A163:B163"/>
-    <mergeCell ref="A164:B164"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="A185:B185"/>
-    <mergeCell ref="A178:B178"/>
-    <mergeCell ref="C80:Y80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C71:Y71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C60:Y60"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="Q13:W13"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="F37:M37"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="F47:M47"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="T9:W9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.98425196850393704" right="0.51181102362204722" top="0.74803149606299213" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.51181102362204722"/>
@@ -44081,15 +44082,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001821B2EC25D39140BA1AC3A0F93B26A5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b58428e78da37c37572897deebd74128">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -44138,6 +44130,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
   <ds:schemaRefs>
@@ -44153,14 +44154,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EECD6A4-5CAC-4EB2-BF99-66BCF0600A47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44173,4 +44166,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>